<commit_message>
Move charts to dedicated sheets and fix Dashboard subtitle formula
- Extract DEBMM Tier Scores chart to its own "Tier Scores Chart" tab
- Extract Organizational Readiness chart to its own "Readiness Chart" tab
- Each chart tab has a visible data table with cross-sheet references
- Remove hidden columns M-P from Results Dashboard
- Fix subtitle formula: leading spaces before = prevented evaluation

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/debmm-assessment.xlsx
+++ b/templates/debmm-assessment.xlsx
@@ -10,8 +10,10 @@
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Assessment" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Results Dashboard" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Rubric Reference" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Report Data" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Tier Scores Chart" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Readiness Chart" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Rubric Reference" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Report Data" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -270,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -324,9 +326,6 @@
     <xf numFmtId="164" fontId="5" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -375,7 +374,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -416,6 +414,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -470,9 +474,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -611,7 +612,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Results Dashboard'!N2</f>
+              <f>'Tier Scores Chart'!C4</f>
             </strRef>
           </tx>
           <spPr>
@@ -676,12 +677,12 @@
           </dPt>
           <cat>
             <numRef>
-              <f>'Results Dashboard'!$M$3:$M$7</f>
+              <f>'Tier Scores Chart'!$B$5:$B$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Results Dashboard'!$N$3:$N$7</f>
+              <f>'Tier Scores Chart'!$C$5:$C$9</f>
             </numRef>
           </val>
         </ser>
@@ -763,7 +764,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Results Dashboard'!P2</f>
+              <f>'Readiness Chart'!C4</f>
             </strRef>
           </tx>
           <spPr>
@@ -795,12 +796,12 @@
           </dPt>
           <cat>
             <numRef>
-              <f>'Results Dashboard'!$O$3:$O$4</f>
+              <f>'Readiness Chart'!$B$5:$B$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Results Dashboard'!$P$3:$P$4</f>
+              <f>'Readiness Chart'!$C$5:$C$6</f>
             </numRef>
           </val>
         </ser>
@@ -860,10 +861,10 @@
     <from>
       <col>1</col>
       <colOff>0</colOff>
-      <row>48</row>
+      <row>10</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6480000" cy="4680000"/>
+    <ext cx="7920000" cy="5040000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -878,23 +879,28 @@
     </graphicFrame>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>4</col>
+      <col>1</col>
       <colOff>0</colOff>
-      <row>48</row>
+      <row>7</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="4320000" cy="4680000"/>
+    <ext cx="6480000" cy="5040000"/>
     <graphicFrame>
       <nvGraphicFramePr>
-        <cNvPr id="2" name="Chart 2"/>
+        <cNvPr id="1" name="Chart 1"/>
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1220,7 +1226,7 @@
     <row r="2" ht="26" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Detection Engineering Behavior Maturity Model — Audit Assessment</t>
+          <t xml:space="preserve">  Detection Engineering Behavior Maturity Model — Self-Assessment</t>
         </is>
       </c>
       <c r="B2" s="4" t="n"/>
@@ -1618,7 +1624,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
@@ -1633,8 +1639,7 @@
     <col width="78" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="45" customWidth="1" min="7" max="7"/>
-    <col width="2" customWidth="1" min="8" max="8"/>
+    <col width="2" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="52" customHeight="1">
@@ -1649,7 +1654,6 @@
       <c r="E1" s="2" t="n"/>
       <c r="F1" s="2" t="n"/>
       <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
     </row>
     <row r="2" ht="24" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
@@ -1663,7 +1667,6 @@
       <c r="E2" s="4" t="n"/>
       <c r="F2" s="4" t="n"/>
       <c r="G2" s="4" t="n"/>
-      <c r="H2" s="4" t="n"/>
     </row>
     <row r="3" ht="8" customHeight="1"/>
     <row r="4">
@@ -1710,7 +1713,7 @@
       </c>
       <c r="D8" s="11" t="inlineStr">
         <is>
-          <t>Audit</t>
+          <t>Self-Assessment</t>
         </is>
       </c>
       <c r="E8" s="12" t="n"/>
@@ -1763,11 +1766,6 @@
           <t>Score</t>
         </is>
       </c>
-      <c r="G12" s="14" t="inlineStr">
-        <is>
-          <t>Evidence / Notes</t>
-        </is>
-      </c>
     </row>
     <row r="13" ht="34" customHeight="1">
       <c r="B13" s="15" t="inlineStr">
@@ -1779,7 +1777,6 @@
       <c r="D13" s="4" t="n"/>
       <c r="E13" s="4" t="n"/>
       <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="n"/>
     </row>
     <row r="14" ht="20" customHeight="1">
       <c r="B14" s="13" t="inlineStr">
@@ -1805,7 +1802,7 @@
       </c>
       <c r="D15" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's rule development process.
+          <t>Rate the maturity of your team's rule development process.
 1 — No structured approach; rules created ad hoc or reactively (0% follow a formal process)
 2 — Some rules follow a loose process but it is inconsistently applied (&lt;30% follow a documented process)
 3 — Defined methodology is documented and followed for most new rules (50-70% follow process; schema alignment &gt;60%)
@@ -1818,30 +1815,28 @@
         <f>IF(E15="","",E15)</f>
         <v/>
       </c>
-      <c r="G15" s="21" t="n"/>
     </row>
     <row r="16" ht="35" customHeight="1">
-      <c r="B16" s="22" t="inlineStr">
+      <c r="B16" s="21" t="inlineStr">
         <is>
           <t>T0-Q2</t>
         </is>
       </c>
-      <c r="C16" s="23" t="inlineStr">
+      <c r="C16" s="22" t="inlineStr">
         <is>
           <t>Structured Rule Development Approach</t>
         </is>
       </c>
-      <c r="D16" s="24" t="inlineStr">
-        <is>
-          <t>Do all new detection rules go through peer review before production deployment?</t>
+      <c r="D16" s="23" t="inlineStr">
+        <is>
+          <t>Do all new detection rules go through peer review before deployment to production?</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
-      <c r="F16" s="25">
+      <c r="F16" s="24">
         <f>IF(E16="Yes",4,IF(E16="No",1,""))</f>
         <v/>
       </c>
-      <c r="G16" s="21" t="n"/>
     </row>
     <row r="17" ht="115" customHeight="1">
       <c r="B17" s="16" t="inlineStr">
@@ -1856,7 +1851,7 @@
       </c>
       <c r="D17" s="18" t="inlineStr">
         <is>
-          <t>What percentage of the assessed team's rules are reviewed on a regular schedule?
+          <t>What percentage of your detection rules are reviewed on a regular schedule?
 1 — Less than 50% reviewed annually; no rule owners assigned
 2 — 50-70% reviewed annually; rules may have informal owners but no formal peer review process
 3 — 70-80% reviewed on schedule; rules have assigned owners and defined review cycles; peer review on most changes
@@ -1869,22 +1864,21 @@
         <f>IF(E17="","",E17)</f>
         <v/>
       </c>
-      <c r="G17" s="21" t="n"/>
     </row>
     <row r="18" ht="115" customHeight="1">
-      <c r="B18" s="22" t="inlineStr">
+      <c r="B18" s="21" t="inlineStr">
         <is>
           <t>T0-Q4</t>
         </is>
       </c>
-      <c r="C18" s="26" t="inlineStr">
+      <c r="C18" s="25" t="inlineStr">
         <is>
           <t>Roadmap Documentation</t>
         </is>
       </c>
-      <c r="D18" s="24" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's detection engineering roadmap.
+      <c r="D18" s="23" t="inlineStr">
+        <is>
+          <t>Rate the maturity of your detection engineering roadmap.
 1 — No roadmap exists; work is entirely reactive or driven by individual initiative
 2 — Informal roadmap or backlog exists (e.g., a Jira board or wiki page) but is not regularly maintained or shared (&lt;30% of work tied to a plan)
 3 — Formal roadmap documented, reviewed at least quarterly, shared with stakeholders; priorities are clear (50-70% of planned work tracked)
@@ -1893,11 +1887,10 @@
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
-      <c r="F18" s="25">
+      <c r="F18" s="24">
         <f>IF(E18="","",E18)</f>
         <v/>
       </c>
-      <c r="G18" s="21" t="n"/>
     </row>
     <row r="19" ht="115" customHeight="1">
       <c r="B19" s="16" t="inlineStr">
@@ -1912,7 +1905,7 @@
       </c>
       <c r="D19" s="18" t="inlineStr">
         <is>
-          <t>How frequently does the assessed team perform threat modeling?
+          <t>How frequently does your team perform threat modeling to inform detection priorities?
 1 — Never performed or not at all
 2 — Less than once per year; typically triggered by a major incident or audit finding
 3 — 1-2 times per year with documented results that inform the detection roadmap
@@ -1925,30 +1918,28 @@
         <f>IF(E19="","",E19)</f>
         <v/>
       </c>
-      <c r="G19" s="21" t="n"/>
     </row>
     <row r="20" ht="35" customHeight="1">
-      <c r="B20" s="22" t="inlineStr">
+      <c r="B20" s="21" t="inlineStr">
         <is>
           <t>T0-Q6</t>
         </is>
       </c>
-      <c r="C20" s="23" t="inlineStr">
+      <c r="C20" s="22" t="inlineStr">
         <is>
           <t>Threat Modeling</t>
         </is>
       </c>
-      <c r="D20" s="24" t="inlineStr">
-        <is>
-          <t>Does the assessed team's threat modeling use a recognized framework?</t>
+      <c r="D20" s="23" t="inlineStr">
+        <is>
+          <t>Does your threat modeling use a recognized framework (e.g., STRIDE, MITRE ATT&amp;CK, PASTA, attack trees)?</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
-      <c r="F20" s="25">
+      <c r="F20" s="24">
         <f>IF(E20="Yes",3,IF(E20="No",1,""))</f>
         <v/>
       </c>
-      <c r="G20" s="21" t="n"/>
     </row>
     <row r="21" ht="35" customHeight="1">
       <c r="B21" s="16" t="inlineStr">
@@ -1956,14 +1947,14 @@
           <t>T0-Q7</t>
         </is>
       </c>
-      <c r="C21" s="27" t="inlineStr">
+      <c r="C21" s="26" t="inlineStr">
         <is>
           <t>Threat Modeling</t>
         </is>
       </c>
       <c r="D21" s="18" t="inlineStr">
         <is>
-          <t>Do threat modeling outputs directly generate items on the assessed team's backlog?</t>
+          <t>Do threat modeling outputs directly generate items on your detection engineering backlog or roadmap?</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -1971,7 +1962,6 @@
         <f>IF(E21="Yes",4,IF(E21="No",1,""))</f>
         <v/>
       </c>
-      <c r="G21" s="21" t="n"/>
     </row>
     <row r="22" ht="34" customHeight="1">
       <c r="B22" s="15" t="inlineStr">
@@ -1983,7 +1973,6 @@
       <c r="D22" s="4" t="n"/>
       <c r="E22" s="4" t="n"/>
       <c r="F22" s="4" t="n"/>
-      <c r="G22" s="4" t="n"/>
     </row>
     <row r="23" ht="20" customHeight="1">
       <c r="B23" s="13" t="inlineStr">
@@ -2009,7 +1998,7 @@
       </c>
       <c r="D24" s="18" t="inlineStr">
         <is>
-          <t>How many custom detection rules does the assessed team maintain?
+          <t>How many custom detection rules does your team maintain (excluding vendor defaults)?
 1 — Fewer than 10 custom rules; mostly relying on vendor/out-of-the-box rules
 2 — 10-30 rules covering the most critical threats (e.g., ransomware, credential theft, C2)
 3 — 30-60 rules with a mix of signature-based and behavioral detections across major categories
@@ -2022,22 +2011,21 @@
         <f>IF(E24="","",E24)</f>
         <v/>
       </c>
-      <c r="G24" s="21" t="n"/>
     </row>
     <row r="25" ht="115" customHeight="1">
-      <c r="B25" s="22" t="inlineStr">
+      <c r="B25" s="21" t="inlineStr">
         <is>
           <t>T1-Q2</t>
         </is>
       </c>
-      <c r="C25" s="23" t="inlineStr">
+      <c r="C25" s="22" t="inlineStr">
         <is>
           <t>Baseline Rule Creation</t>
         </is>
       </c>
-      <c r="D25" s="24" t="inlineStr">
-        <is>
-          <t>Estimate the assessed team's MITRE ATT&amp;CK technique coverage for priority areas.
+      <c r="D25" s="23" t="inlineStr">
+        <is>
+          <t>Estimate your MITRE ATT&amp;CK technique coverage for your organization's priority threat areas.
 1 — Unknown or not measured; no ATT&amp;CK mapping performed
 2 — Less than 30% of priority techniques covered; coverage is ad hoc
 3 — 30-50% of priority techniques covered with documented gaps identified
@@ -2046,11 +2034,10 @@
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
-      <c r="F25" s="25">
+      <c r="F25" s="24">
         <f>IF(E25="","",E25)</f>
         <v/>
       </c>
-      <c r="G25" s="21" t="n"/>
     </row>
     <row r="26" ht="115" customHeight="1">
       <c r="B26" s="16" t="inlineStr">
@@ -2065,7 +2052,7 @@
       </c>
       <c r="D26" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's ruleset management.
+          <t>Rate the maturity of your ruleset management practices.
 1 — No formal management; rules live only in the SIEM console with no version control or documentation (&lt;20% in version control)
 2 — Some rules stored in version control (e.g., Git) with basic documentation (20-50% in VCS)
 3 — Most rules in version control with documentation standards; detection-as-code approach being adopted (50-80% in VCS with docs)
@@ -2078,22 +2065,21 @@
         <f>IF(E26="","",E26)</f>
         <v/>
       </c>
-      <c r="G26" s="21" t="n"/>
     </row>
     <row r="27" ht="115" customHeight="1">
-      <c r="B27" s="22" t="inlineStr">
+      <c r="B27" s="21" t="inlineStr">
         <is>
           <t>T1-Q4</t>
         </is>
       </c>
-      <c r="C27" s="26" t="inlineStr">
+      <c r="C27" s="25" t="inlineStr">
         <is>
           <t>Telemetry Quality</t>
         </is>
       </c>
-      <c r="D27" s="24" t="inlineStr">
-        <is>
-          <t>Rate the quality and coverage of the assessed team's telemetry.
+      <c r="D27" s="23" t="inlineStr">
+        <is>
+          <t>Rate the quality and coverage of your telemetry data sources for detection.
 1 — No active telemetry management; using whatever data sources happen to be available (&lt;30% of rule types have adequate telemetry)
 2 — Some awareness of gaps; basic health checks on critical sources like EDR and firewall logs (30-50% adequate coverage)
 3 — Actively monitored; data source coverage mapped to detection needs; CTI enrichment beginning (50-70% coverage)
@@ -2102,11 +2088,10 @@
         </is>
       </c>
       <c r="E27" s="19" t="n"/>
-      <c r="F27" s="25">
+      <c r="F27" s="24">
         <f>IF(E27="","",E27)</f>
         <v/>
       </c>
-      <c r="G27" s="21" t="n"/>
     </row>
     <row r="28" ht="35" customHeight="1">
       <c r="B28" s="16" t="inlineStr">
@@ -2114,14 +2099,14 @@
           <t>T1-Q5</t>
         </is>
       </c>
-      <c r="C28" s="27" t="inlineStr">
+      <c r="C28" s="26" t="inlineStr">
         <is>
           <t>Telemetry Quality</t>
         </is>
       </c>
       <c r="D28" s="18" t="inlineStr">
         <is>
-          <t>Does the assessed team maintain a documented data source inventory mapped to use cases?</t>
+          <t>Do you maintain a documented inventory of telemetry data sources mapped to detection use cases?</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -2129,30 +2114,28 @@
         <f>IF(E28="Yes",3,IF(E28="No",1,""))</f>
         <v/>
       </c>
-      <c r="G28" s="21" t="n"/>
     </row>
     <row r="29" ht="35" customHeight="1">
-      <c r="B29" s="22" t="inlineStr">
+      <c r="B29" s="21" t="inlineStr">
         <is>
           <t>T1-Q6</t>
         </is>
       </c>
-      <c r="C29" s="23" t="inlineStr">
+      <c r="C29" s="22" t="inlineStr">
         <is>
           <t>Telemetry Quality</t>
         </is>
       </c>
-      <c r="D29" s="24" t="inlineStr">
-        <is>
-          <t>Does the assessed team have automated alerting for data source degradation?</t>
+      <c r="D29" s="23" t="inlineStr">
+        <is>
+          <t>Do you have automated alerting for when critical data sources stop ingesting or degrade in quality?</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
-      <c r="F29" s="25">
+      <c r="F29" s="24">
         <f>IF(E29="Yes",4,IF(E29="No",1,""))</f>
         <v/>
       </c>
-      <c r="G29" s="21" t="n"/>
     </row>
     <row r="30" ht="115" customHeight="1">
       <c r="B30" s="16" t="inlineStr">
@@ -2167,7 +2150,7 @@
       </c>
       <c r="D30" s="18" t="inlineStr">
         <is>
-          <t>How frequently does the assessed team review the threat landscape?
+          <t>How frequently does your team review the threat landscape to update detection priorities?
 1 — No regular reviews; detection priorities are not informed by current threats
 2 — Annually or bi-annually; some rule updates after major threat advisories (1-2 reviews/year)
 3 — Quarterly with documented findings that update the detection roadmap (50-70% of rules reviewed against current threats)
@@ -2180,22 +2163,21 @@
         <f>IF(E30="","",E30)</f>
         <v/>
       </c>
-      <c r="G30" s="21" t="n"/>
     </row>
     <row r="31" ht="115" customHeight="1">
-      <c r="B31" s="22" t="inlineStr">
+      <c r="B31" s="21" t="inlineStr">
         <is>
           <t>T1-Q8</t>
         </is>
       </c>
-      <c r="C31" s="26" t="inlineStr">
+      <c r="C31" s="25" t="inlineStr">
         <is>
           <t>Product Owner Engagement</t>
         </is>
       </c>
-      <c r="D31" s="24" t="inlineStr">
-        <is>
-          <t>Rate the engagement between the assessed team and product/platform owners.
+      <c r="D31" s="23" t="inlineStr">
+        <is>
+          <t>Rate the engagement between your detection engineering team and security product/platform owners (e.g., SIEM vendor, EDR team).
 1 — No engagement; detection needs are never communicated to product/platform teams
 2 — Occasional ad hoc engagement, typically reactive to issues or missing features (fewer than 4 interactions per year)
 3 — Quarterly structured engagements to communicate detection needs, request features, and provide feedback
@@ -2204,11 +2186,10 @@
         </is>
       </c>
       <c r="E31" s="19" t="n"/>
-      <c r="F31" s="25">
+      <c r="F31" s="24">
         <f>IF(E31="","",E31)</f>
         <v/>
       </c>
-      <c r="G31" s="21" t="n"/>
     </row>
     <row r="32" ht="115" customHeight="1">
       <c r="B32" s="16" t="inlineStr">
@@ -2223,7 +2204,7 @@
       </c>
       <c r="D32" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's release testing.
+          <t>Rate the maturity of your detection rule testing before production deployment.
 1 — No testing; rules are deployed to production without validation (&lt;20% tested)
 2 — Basic manual testing on some rules before deployment; no standardized process or test environment (20-40% tested)
 3 — Standardized testing with defined test cases and a staging/test environment; most rules validated before deploy (50-70% tested)
@@ -2236,7 +2217,6 @@
         <f>IF(E32="","",E32)</f>
         <v/>
       </c>
-      <c r="G32" s="21" t="n"/>
     </row>
     <row r="33" ht="34" customHeight="1">
       <c r="B33" s="15" t="inlineStr">
@@ -2248,7 +2228,6 @@
       <c r="D33" s="4" t="n"/>
       <c r="E33" s="4" t="n"/>
       <c r="F33" s="4" t="n"/>
-      <c r="G33" s="4" t="n"/>
     </row>
     <row r="34" ht="20" customHeight="1">
       <c r="B34" s="13" t="inlineStr">
@@ -2274,7 +2253,7 @@
       </c>
       <c r="D35" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's FP reduction program.
+          <t>Rate the maturity of your false positive tuning and reduction program.
 1 — Minimal or no tuning; high false positive rates accepted as normal; no FP metrics tracked
 2 — Reactive tuning when analysts complain about noisy rules; no systematic tracking of FP rates (10-25% FP reduction from baseline)
 3 — Regular tuning cycles (at least quarterly); FP rates tracked per rule; tuning is documented (25-50% FP reduction)
@@ -2287,22 +2266,21 @@
         <f>IF(E35="","",E35)</f>
         <v/>
       </c>
-      <c r="G35" s="21" t="n"/>
     </row>
     <row r="36" ht="115" customHeight="1">
-      <c r="B36" s="22" t="inlineStr">
+      <c r="B36" s="21" t="inlineStr">
         <is>
           <t>T2-Q2</t>
         </is>
       </c>
-      <c r="C36" s="23" t="inlineStr">
+      <c r="C36" s="22" t="inlineStr">
         <is>
           <t>False Positive Tuning and Reduction</t>
         </is>
       </c>
-      <c r="D36" s="24" t="inlineStr">
-        <is>
-          <t>What is the assessed team's estimated FP reduction from baseline?
+      <c r="D36" s="23" t="inlineStr">
+        <is>
+          <t>What is your estimated false positive reduction from initial baseline across your tuned rules?
 1 — Unknown or not measured
 2 — Less than 25% reduction
 3 — 25-50% reduction with per-rule FP rate tracking
@@ -2311,11 +2289,10 @@
         </is>
       </c>
       <c r="E36" s="19" t="n"/>
-      <c r="F36" s="25">
+      <c r="F36" s="24">
         <f>IF(E36="","",E36)</f>
         <v/>
       </c>
-      <c r="G36" s="21" t="n"/>
     </row>
     <row r="37" ht="115" customHeight="1">
       <c r="B37" s="16" t="inlineStr">
@@ -2330,7 +2307,7 @@
       </c>
       <c r="D37" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's gap analysis.
+          <t>Rate the maturity of your detection coverage gap analysis.
 1 — No gap analysis performed; detection coverage gaps are unknown
 2 — Some gaps identified informally after incidents expose missing detections (1-3 gaps documented; reactive only)
 3 — Regular analysis against ATT&amp;CK or similar frameworks at least quarterly; gaps documented, prioritized, and tracked (5+ gaps documented and prioritized)
@@ -2343,30 +2320,28 @@
         <f>IF(E37="","",E37)</f>
         <v/>
       </c>
-      <c r="G37" s="21" t="n"/>
     </row>
     <row r="38" ht="35" customHeight="1">
-      <c r="B38" s="22" t="inlineStr">
+      <c r="B38" s="21" t="inlineStr">
         <is>
           <t>T2-Q4</t>
         </is>
       </c>
-      <c r="C38" s="23" t="inlineStr">
+      <c r="C38" s="22" t="inlineStr">
         <is>
           <t>Gap Analysis and Documentation</t>
         </is>
       </c>
-      <c r="D38" s="24" t="inlineStr">
-        <is>
-          <t>Does the assessed team maintain a documented, prioritized gap list updated quarterly?</t>
+      <c r="D38" s="23" t="inlineStr">
+        <is>
+          <t>Do you maintain a documented, prioritized list of detection coverage gaps that is updated at least quarterly?</t>
         </is>
       </c>
       <c r="E38" s="19" t="n"/>
-      <c r="F38" s="25">
+      <c r="F38" s="24">
         <f>IF(E38="Yes",3,IF(E38="No",1,""))</f>
         <v/>
       </c>
-      <c r="G38" s="21" t="n"/>
     </row>
     <row r="39" ht="35" customHeight="1">
       <c r="B39" s="16" t="inlineStr">
@@ -2374,14 +2349,14 @@
           <t>T2-Q5</t>
         </is>
       </c>
-      <c r="C39" s="27" t="inlineStr">
+      <c r="C39" s="26" t="inlineStr">
         <is>
           <t>Gap Analysis and Documentation</t>
         </is>
       </c>
       <c r="D39" s="18" t="inlineStr">
         <is>
-          <t>Are the assessed team's gaps communicated to stakeholders at least quarterly?</t>
+          <t>Are detection coverage gaps formally communicated to stakeholders (leadership, IR, threat intel) at least quarterly?</t>
         </is>
       </c>
       <c r="E39" s="19" t="n"/>
@@ -2389,22 +2364,21 @@
         <f>IF(E39="Yes",4,IF(E39="No",1,""))</f>
         <v/>
       </c>
-      <c r="G39" s="21" t="n"/>
     </row>
     <row r="40" ht="115" customHeight="1">
-      <c r="B40" s="22" t="inlineStr">
+      <c r="B40" s="21" t="inlineStr">
         <is>
           <t>T2-Q6</t>
         </is>
       </c>
-      <c r="C40" s="26" t="inlineStr">
+      <c r="C40" s="25" t="inlineStr">
         <is>
           <t>Internal Testing and Validation</t>
         </is>
       </c>
-      <c r="D40" s="24" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's internal testing program.
+      <c r="D40" s="23" t="inlineStr">
+        <is>
+          <t>Rate the maturity of your internal detection testing and validation program.
 1 — No internal testing; rules are assumed to work once deployed
 2 — Occasional manual testing of high-priority rules using basic atomic tests (&lt;40% emulation coverage)
 3 — Regular testing program with attack emulation (e.g., Atomic Red Team, Caldera) covering major detection categories; results documented (40-70% emulation coverage; at least quarterly)
@@ -2413,11 +2387,10 @@
         </is>
       </c>
       <c r="E40" s="19" t="n"/>
-      <c r="F40" s="25">
+      <c r="F40" s="24">
         <f>IF(E40="","",E40)</f>
         <v/>
       </c>
-      <c r="G40" s="21" t="n"/>
     </row>
     <row r="41" ht="34" customHeight="1">
       <c r="B41" s="15" t="inlineStr">
@@ -2429,7 +2402,6 @@
       <c r="D41" s="4" t="n"/>
       <c r="E41" s="4" t="n"/>
       <c r="F41" s="4" t="n"/>
-      <c r="G41" s="4" t="n"/>
     </row>
     <row r="42" ht="20" customHeight="1">
       <c r="B42" s="13" t="inlineStr">
@@ -2455,7 +2427,7 @@
       </c>
       <c r="D43" s="18" t="inlineStr">
         <is>
-          <t>Rate the assessed team's ability to detect and remediate false negatives.
+          <t>Rate your team's ability to identify and remediate false negatives (missed detections).
 1 — No FN identification process; missed detections only discovered during incident response
 2 — Some FNs identified through post-incident reviews; basic tracking of missed detections (50% of tested samples trigger expected alerts)
 3 — Systematic FN identification through regular testing and validation; root causes analyzed and documented (70-90% trigger rate; 30-50% FN reduction)
@@ -2468,22 +2440,21 @@
         <f>IF(E43="","",E43)</f>
         <v/>
       </c>
-      <c r="G43" s="21" t="n"/>
     </row>
     <row r="44" ht="115" customHeight="1">
-      <c r="B44" s="22" t="inlineStr">
+      <c r="B44" s="21" t="inlineStr">
         <is>
           <t>T3-Q2</t>
         </is>
       </c>
-      <c r="C44" s="23" t="inlineStr">
+      <c r="C44" s="22" t="inlineStr">
         <is>
           <t>False Negative Triage</t>
         </is>
       </c>
-      <c r="D44" s="24" t="inlineStr">
-        <is>
-          <t>What is the assessed team's detection trigger rate on tested samples?
+      <c r="D44" s="23" t="inlineStr">
+        <is>
+          <t>What is your detection trigger rate when tested samples or emulations are run against your rules?
 1 — Unknown or not tested
 2 — Less than 50% of test samples trigger expected detections
 3 — 50-70% trigger rate with root cause analysis on misses
@@ -2492,11 +2463,10 @@
         </is>
       </c>
       <c r="E44" s="19" t="n"/>
-      <c r="F44" s="25">
+      <c r="F44" s="24">
         <f>IF(E44="","",E44)</f>
         <v/>
       </c>
-      <c r="G44" s="21" t="n"/>
     </row>
     <row r="45" ht="115" customHeight="1">
       <c r="B45" s="16" t="inlineStr">
@@ -2511,7 +2481,7 @@
       </c>
       <c r="D45" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's external validation.
+          <t>Rate the maturity of your external validation program for detection capabilities.
 1 — No external validation; no red team, pentest, or third-party assessment of detection effectiveness
 2 — Annual penetration test that includes some detection assessment but is not detection-focused (1 exercise per year)
 3 — Regular external validation through red team engagements or third-party assessments specifically focused on detection effectiveness (&gt;1 per year; findings drive improvements)
@@ -2524,22 +2494,21 @@
         <f>IF(E45="","",E45)</f>
         <v/>
       </c>
-      <c r="G45" s="21" t="n"/>
     </row>
     <row r="46" ht="115" customHeight="1">
-      <c r="B46" s="22" t="inlineStr">
+      <c r="B46" s="21" t="inlineStr">
         <is>
           <t>T3-Q4</t>
         </is>
       </c>
-      <c r="C46" s="26" t="inlineStr">
+      <c r="C46" s="25" t="inlineStr">
         <is>
           <t>Advanced TTP Coverage</t>
         </is>
       </c>
-      <c r="D46" s="24" t="inlineStr">
-        <is>
-          <t>Rate the assessed team's coverage of advanced TTPs.
+      <c r="D46" s="23" t="inlineStr">
+        <is>
+          <t>Rate your detection coverage of advanced TTPs beyond basic signatures and IOCs.
 1 — No advanced TTP coverage; detections are signature/IOC-based only
 2 — Limited coverage of 1-2 advanced technique categories (e.g., basic PowerShell abuse detection)
 3 — Growing coverage of 3-4 categories informed by threat intel; behavioral detections supplement signatures (e.g., LOLBin usage, fileless execution, credential access evasion)
@@ -2548,11 +2517,10 @@
         </is>
       </c>
       <c r="E46" s="19" t="n"/>
-      <c r="F46" s="25">
+      <c r="F46" s="24">
         <f>IF(E46="","",E46)</f>
         <v/>
       </c>
-      <c r="G46" s="21" t="n"/>
     </row>
     <row r="47" ht="115" customHeight="1">
       <c r="B47" s="16" t="inlineStr">
@@ -2560,14 +2528,14 @@
           <t>T3-Q5</t>
         </is>
       </c>
-      <c r="C47" s="27" t="inlineStr">
+      <c r="C47" s="26" t="inlineStr">
         <is>
           <t>Advanced TTP Coverage</t>
         </is>
       </c>
       <c r="D47" s="18" t="inlineStr">
         <is>
-          <t>How many of these categories does the assessed team have behavioral detections for: LOLBins, fileless malware, credential evasion, defense evasion, lateral movement?
+          <t>How many of these advanced TTP categories does your team have behavioral detections for: (1) LOLBins/living-off-the-land, (2) fileless malware, (3) credential dumping evasion, (4) defense evasion/log tampering, (5) lateral movement via legitimate tools?
 1 — None of these
 2 — 1 of these categories
 3 — 2-3 of these categories
@@ -2580,7 +2548,6 @@
         <f>IF(E47="","",E47)</f>
         <v/>
       </c>
-      <c r="G47" s="21" t="n"/>
     </row>
     <row r="48" ht="34" customHeight="1">
       <c r="B48" s="15" t="inlineStr">
@@ -2592,7 +2559,6 @@
       <c r="D48" s="4" t="n"/>
       <c r="E48" s="4" t="n"/>
       <c r="F48" s="4" t="n"/>
-      <c r="G48" s="4" t="n"/>
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="B49" s="13" t="inlineStr">
@@ -2618,7 +2584,7 @@
       </c>
       <c r="D50" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's threat hunting.
+          <t>Rate the maturity of your threat hunting program.
 1 — No proactive hunting; all detection is passive through deployed rules
 2 — Occasional ad hoc hunting triggered by intel or incidents; findings not systematically converted to detections (fewer than 2 hunts/month; &lt;30% findings converted to rules)
 3 — Regular structured hunting at least weekly, driven by documented hypotheses from intel or gap analysis; findings feed detection development (weekly hunts; 50-70% of findings integrated into rules)
@@ -2631,30 +2597,28 @@
         <f>IF(E50="","",E50)</f>
         <v/>
       </c>
-      <c r="G50" s="21" t="n"/>
     </row>
     <row r="51" ht="35" customHeight="1">
-      <c r="B51" s="22" t="inlineStr">
+      <c r="B51" s="21" t="inlineStr">
         <is>
           <t>T4-Q2</t>
         </is>
       </c>
-      <c r="C51" s="23" t="inlineStr">
+      <c r="C51" s="22" t="inlineStr">
         <is>
           <t>Threat Hunting in Telemetry</t>
         </is>
       </c>
-      <c r="D51" s="24" t="inlineStr">
-        <is>
-          <t>Are the assessed team's hunts driven by documented hypotheses?</t>
+      <c r="D51" s="23" t="inlineStr">
+        <is>
+          <t>Are your threat hunts driven by documented hypotheses (from intel, incidents, or gap analysis) rather than ad hoc exploration?</t>
         </is>
       </c>
       <c r="E51" s="19" t="n"/>
-      <c r="F51" s="25">
+      <c r="F51" s="24">
         <f>IF(E51="Yes",4,IF(E51="No",1,""))</f>
         <v/>
       </c>
-      <c r="G51" s="21" t="n"/>
     </row>
     <row r="52" ht="35" customHeight="1">
       <c r="B52" s="16" t="inlineStr">
@@ -2662,14 +2626,14 @@
           <t>T4-Q3</t>
         </is>
       </c>
-      <c r="C52" s="27" t="inlineStr">
+      <c r="C52" s="26" t="inlineStr">
         <is>
           <t>Threat Hunting in Telemetry</t>
         </is>
       </c>
       <c r="D52" s="18" t="inlineStr">
         <is>
-          <t>Is there a defined process to convert hunting findings into production rules?</t>
+          <t>Is there a defined process to convert threat hunting findings into production detection rules?</t>
         </is>
       </c>
       <c r="E52" s="19" t="n"/>
@@ -2677,22 +2641,21 @@
         <f>IF(E52="Yes",4,IF(E52="No",1,""))</f>
         <v/>
       </c>
-      <c r="G52" s="21" t="n"/>
     </row>
     <row r="53" ht="115" customHeight="1">
-      <c r="B53" s="22" t="inlineStr">
+      <c r="B53" s="21" t="inlineStr">
         <is>
           <t>T4-Q4</t>
         </is>
       </c>
-      <c r="C53" s="26" t="inlineStr">
+      <c r="C53" s="25" t="inlineStr">
         <is>
           <t>Automation and Continuous Improvement</t>
         </is>
       </c>
-      <c r="D53" s="24" t="inlineStr">
-        <is>
-          <t>What percentage of the assessed team's DE tasks are automated?
+      <c r="D53" s="23" t="inlineStr">
+        <is>
+          <t>What percentage of your detection engineering tasks are automated?
 1 — None; all processes are manual (0% automated)
 2 — Basic automation of some repetitive tasks like deployment scripts (&lt;30% automated)
 3 — Significant lifecycle automation including AI-based quality checks on new rules; improvement metrics tracked (40-60% automated)
@@ -2701,11 +2664,10 @@
         </is>
       </c>
       <c r="E53" s="19" t="n"/>
-      <c r="F53" s="25">
+      <c r="F53" s="24">
         <f>IF(E53="","",E53)</f>
         <v/>
       </c>
-      <c r="G53" s="21" t="n"/>
     </row>
     <row r="54" ht="115" customHeight="1">
       <c r="B54" s="16" t="inlineStr">
@@ -2713,14 +2675,14 @@
           <t>T4-Q5</t>
         </is>
       </c>
-      <c r="C54" s="27" t="inlineStr">
+      <c r="C54" s="26" t="inlineStr">
         <is>
           <t>Automation and Continuous Improvement</t>
         </is>
       </c>
       <c r="D54" s="18" t="inlineStr">
         <is>
-          <t>How many detection lifecycle stages have automation or AI integration?
+          <t>How many detection lifecycle stages have AI/LLM or automation integration? Stages: (1) rule authoring, (2) testing, (3) tuning, (4) deployment, (5) monitoring, (6) retirement.
 1 — None; all stages are manual
 2 — 1 stage (e.g., deployment scripts only)
 3 — 2-3 stages automated or AI-assisted
@@ -2733,94 +2695,86 @@
         <f>IF(E54="","",E54)</f>
         <v/>
       </c>
-      <c r="G54" s="21" t="n"/>
     </row>
     <row r="55" ht="20" customHeight="1">
-      <c r="A55" s="28" t="n"/>
-      <c r="B55" s="28" t="n"/>
-      <c r="C55" s="28" t="n"/>
-      <c r="D55" s="28" t="n"/>
-      <c r="E55" s="28" t="n"/>
-      <c r="F55" s="28" t="n"/>
-      <c r="G55" s="28" t="n"/>
-      <c r="H55" s="28" t="n"/>
+      <c r="A55" s="27" t="n"/>
+      <c r="B55" s="27" t="n"/>
+      <c r="C55" s="27" t="n"/>
+      <c r="D55" s="27" t="n"/>
+      <c r="E55" s="27" t="n"/>
+      <c r="F55" s="27" t="n"/>
+      <c r="G55" s="27" t="n"/>
     </row>
     <row r="56" ht="32" customHeight="1">
-      <c r="B56" s="29" t="inlineStr">
+      <c r="B56" s="28" t="inlineStr">
         <is>
           <t>SUPPLEMENTARY DIMENSIONS — Organizational Readiness</t>
         </is>
       </c>
-      <c r="C56" s="30" t="n"/>
-      <c r="D56" s="30" t="n"/>
-      <c r="E56" s="30" t="n"/>
-      <c r="F56" s="30" t="n"/>
+      <c r="C56" s="29" t="n"/>
+      <c r="D56" s="29" t="n"/>
+      <c r="E56" s="29" t="n"/>
+      <c r="F56" s="29" t="n"/>
     </row>
     <row r="57" ht="22" customHeight="1">
-      <c r="B57" s="31" t="inlineStr">
+      <c r="B57" s="30" t="inlineStr">
         <is>
           <t>These dimensions from detectionengineering.io assess people and process factors. They contribute to the overall score but do not affect DEBMM tier determination.</t>
         </is>
       </c>
-      <c r="C57" s="30" t="n"/>
-      <c r="D57" s="30" t="n"/>
-      <c r="E57" s="30" t="n"/>
-      <c r="F57" s="30" t="n"/>
+      <c r="C57" s="29" t="n"/>
+      <c r="D57" s="29" t="n"/>
+      <c r="E57" s="29" t="n"/>
+      <c r="F57" s="29" t="n"/>
     </row>
     <row r="58" ht="26" customHeight="1">
-      <c r="B58" s="32" t="inlineStr">
+      <c r="B58" s="31" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C58" s="32" t="inlineStr">
+      <c r="C58" s="31" t="inlineStr">
         <is>
           <t>Criterion</t>
         </is>
       </c>
-      <c r="D58" s="32" t="inlineStr">
+      <c r="D58" s="31" t="inlineStr">
         <is>
           <t>Question</t>
         </is>
       </c>
-      <c r="E58" s="32" t="inlineStr">
+      <c r="E58" s="31" t="inlineStr">
         <is>
           <t>Answer</t>
         </is>
       </c>
-      <c r="F58" s="32" t="inlineStr">
+      <c r="F58" s="31" t="inlineStr">
         <is>
           <t>Score</t>
         </is>
       </c>
-      <c r="G58" s="32" t="inlineStr">
-        <is>
-          <t>Evidence / Notes</t>
-        </is>
-      </c>
     </row>
     <row r="59" ht="34" customHeight="1">
-      <c r="B59" s="33" t="inlineStr">
+      <c r="B59" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">  PEOPLE &amp; ORGANIZATION</t>
         </is>
       </c>
-      <c r="C59" s="34" t="n"/>
-      <c r="D59" s="34" t="n"/>
-      <c r="E59" s="34" t="n"/>
-      <c r="F59" s="34" t="n"/>
-      <c r="G59" s="34" t="n"/>
+      <c r="C59" s="33" t="n"/>
+      <c r="D59" s="33" t="n"/>
+      <c r="E59" s="33" t="n"/>
+      <c r="F59" s="33" t="n"/>
     </row>
     <row r="60" ht="20" customHeight="1">
-      <c r="B60" s="31" t="inlineStr">
+      <c r="B60" s="30" t="inlineStr">
         <is>
           <t>Assesses the human and organizational factors that enable effective detection engineering, drawn from Kyle Bailey's Detection Engineering Maturity Matrix.</t>
         </is>
       </c>
-      <c r="C60" s="30" t="n"/>
-      <c r="D60" s="30" t="n"/>
-      <c r="E60" s="30" t="n"/>
-      <c r="F60" s="30" t="n"/>
+      <c r="C60" s="29" t="n"/>
+      <c r="D60" s="29" t="n"/>
+      <c r="E60" s="29" t="n"/>
+      <c r="F60" s="29" t="n"/>
     </row>
     <row r="61" ht="115" customHeight="1">
       <c r="B61" s="16" t="inlineStr">
@@ -2835,7 +2789,7 @@
       </c>
       <c r="D61" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed detection engineering team structure.
+          <t>Rate the maturity of your detection engineering team structure.
 1 — No dedicated roles; detection work is a side task for SOC analysts or other staff (0 dedicated FTEs)
 2 — One or more staff have detection engineering as a partial responsibility; no formal team or career path
 3 — At least one dedicated detection engineering role or team established with clear responsibilities and defined career progression
@@ -2848,22 +2802,21 @@
         <f>IF(E61="","",E61)</f>
         <v/>
       </c>
-      <c r="G61" s="21" t="n"/>
     </row>
     <row r="62" ht="115" customHeight="1">
-      <c r="B62" s="35" t="inlineStr">
+      <c r="B62" s="34" t="inlineStr">
         <is>
           <t>EP-Q2</t>
         </is>
       </c>
-      <c r="C62" s="36" t="inlineStr">
+      <c r="C62" s="35" t="inlineStr">
         <is>
           <t>Skills Development and Training</t>
         </is>
       </c>
-      <c r="D62" s="37" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's skills development.
+      <c r="D62" s="36" t="inlineStr">
+        <is>
+          <t>Rate the maturity of your detection engineering skills development program.
 1 — No formal training; learning is entirely self-directed with no organizational support or budget
 2 — Ad hoc training; individuals may attend a conference or take a course occasionally but there is no structured program
 3 — Written training plan with scheduled activities; regular knowledge sharing sessions (e.g., weekly/biweekly); defined skill requirements for roles
@@ -2872,11 +2825,10 @@
         </is>
       </c>
       <c r="E62" s="19" t="n"/>
-      <c r="F62" s="38">
+      <c r="F62" s="37">
         <f>IF(E62="","",E62)</f>
         <v/>
       </c>
-      <c r="G62" s="21" t="n"/>
     </row>
     <row r="63" ht="115" customHeight="1">
       <c r="B63" s="16" t="inlineStr">
@@ -2891,7 +2843,7 @@
       </c>
       <c r="D63" s="18" t="inlineStr">
         <is>
-          <t>Rate the executive sponsorship of the assessed detection engineering function.
+          <t>Rate the level of executive sponsorship and leadership commitment to detection engineering.
 1 — No executive awareness; detection engineering is not recognized as a distinct capability
 2 — Some leadership awareness but no formal executive sponsor, no dedicated budget allocation
 3 — Executive sponsor identified; dedicated budget for tooling and headcount; detection engineering formally recognized as a function
@@ -2904,30 +2856,28 @@
         <f>IF(E63="","",E63)</f>
         <v/>
       </c>
-      <c r="G63" s="21" t="n"/>
     </row>
     <row r="64" ht="35" customHeight="1">
-      <c r="B64" s="35" t="inlineStr">
+      <c r="B64" s="34" t="inlineStr">
         <is>
           <t>EP-Q4</t>
         </is>
       </c>
-      <c r="C64" s="39" t="inlineStr">
+      <c r="C64" s="38" t="inlineStr">
         <is>
           <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
-      <c r="D64" s="37" t="inlineStr">
-        <is>
-          <t>Does the assessed team present metrics to executive leadership at least quarterly?</t>
+      <c r="D64" s="36" t="inlineStr">
+        <is>
+          <t>Does your detection engineering team present metrics or results to executive leadership at least quarterly?</t>
         </is>
       </c>
       <c r="E64" s="19" t="n"/>
-      <c r="F64" s="38">
+      <c r="F64" s="37">
         <f>IF(E64="Yes",3,IF(E64="No",1,""))</f>
         <v/>
       </c>
-      <c r="G64" s="21" t="n"/>
     </row>
     <row r="65" ht="35" customHeight="1">
       <c r="B65" s="16" t="inlineStr">
@@ -2935,14 +2885,14 @@
           <t>EP-Q5</t>
         </is>
       </c>
-      <c r="C65" s="27" t="inlineStr">
+      <c r="C65" s="26" t="inlineStr">
         <is>
           <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
       <c r="D65" s="18" t="inlineStr">
         <is>
-          <t>Has leadership made investment/staffing decisions based on the assessed team's metrics in the past year?</t>
+          <t>Has executive leadership made investment or staffing decisions based on detection engineering metrics or recommendations in the past year?</t>
         </is>
       </c>
       <c r="E65" s="19" t="n"/>
@@ -2950,30 +2900,28 @@
         <f>IF(E65="Yes",4,IF(E65="No",1,""))</f>
         <v/>
       </c>
-      <c r="G65" s="21" t="n"/>
     </row>
     <row r="66" ht="34" customHeight="1">
-      <c r="B66" s="33" t="inlineStr">
+      <c r="B66" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">  PROCESS &amp; GOVERNANCE</t>
         </is>
       </c>
-      <c r="C66" s="34" t="n"/>
-      <c r="D66" s="34" t="n"/>
-      <c r="E66" s="34" t="n"/>
-      <c r="F66" s="34" t="n"/>
-      <c r="G66" s="34" t="n"/>
+      <c r="C66" s="33" t="n"/>
+      <c r="D66" s="33" t="n"/>
+      <c r="E66" s="33" t="n"/>
+      <c r="F66" s="33" t="n"/>
     </row>
     <row r="67" ht="20" customHeight="1">
-      <c r="B67" s="31" t="inlineStr">
+      <c r="B67" s="30" t="inlineStr">
         <is>
           <t>Assesses the process maturity and governance structures supporting detection engineering, drawn from Kyle Bailey's Detection Engineering Maturity Matrix.</t>
         </is>
       </c>
-      <c r="C67" s="30" t="n"/>
-      <c r="D67" s="30" t="n"/>
-      <c r="E67" s="30" t="n"/>
-      <c r="F67" s="30" t="n"/>
+      <c r="C67" s="29" t="n"/>
+      <c r="D67" s="29" t="n"/>
+      <c r="E67" s="29" t="n"/>
+      <c r="F67" s="29" t="n"/>
     </row>
     <row r="68" ht="115" customHeight="1">
       <c r="B68" s="16" t="inlineStr">
@@ -2988,7 +2936,7 @@
       </c>
       <c r="D68" s="18" t="inlineStr">
         <is>
-          <t>Rate the maturity of the assessed team's detection lifecycle workflow.
+          <t>Rate the maturity of your detection lifecycle workflow (from request through retirement).
 1 — No defined lifecycle; detections created and deployed without structured workflow
 2 — Basic lifecycle covering creation and deployment only; no formal stages for review, testing, or retirement (2-3 stages defined)
 3 — Full lifecycle defined and followed: request, development, review, testing, deployment, monitoring, and retirement (all 7 stages documented)
@@ -3001,22 +2949,21 @@
         <f>IF(E68="","",E68)</f>
         <v/>
       </c>
-      <c r="G68" s="21" t="n"/>
     </row>
     <row r="69" ht="115" customHeight="1">
-      <c r="B69" s="35" t="inlineStr">
+      <c r="B69" s="34" t="inlineStr">
         <is>
           <t>EG-Q2</t>
         </is>
       </c>
-      <c r="C69" s="36" t="inlineStr">
+      <c r="C69" s="35" t="inlineStr">
         <is>
           <t>Metrics and KPI Tracking</t>
         </is>
       </c>
-      <c r="D69" s="37" t="inlineStr">
-        <is>
-          <t>Rate the maturity of the assessed team's metrics program.
+      <c r="D69" s="36" t="inlineStr">
+        <is>
+          <t>Rate the maturity of your detection engineering metrics program.
 1 — No metrics tracked; success is anecdotal or unmeasured
 2 — 1-2 basic metrics tracked informally (e.g., rule count, alert volume); no formal KPI program or dashboards
 3 — 3-5 defined KPIs covering key areas with quarterly reporting and dashboards (e.g., coverage %, FP rate, deployment velocity)
@@ -3025,11 +2972,10 @@
         </is>
       </c>
       <c r="E69" s="19" t="n"/>
-      <c r="F69" s="38">
+      <c r="F69" s="37">
         <f>IF(E69="","",E69)</f>
         <v/>
       </c>
-      <c r="G69" s="21" t="n"/>
     </row>
     <row r="70" ht="115" customHeight="1">
       <c r="B70" s="16" t="inlineStr">
@@ -3037,14 +2983,14 @@
           <t>EG-Q3</t>
         </is>
       </c>
-      <c r="C70" s="27" t="inlineStr">
+      <c r="C70" s="26" t="inlineStr">
         <is>
           <t>Metrics and KPI Tracking</t>
         </is>
       </c>
       <c r="D70" s="18" t="inlineStr">
         <is>
-          <t>How many of these KPI categories does the assessed team track: coverage, quality, velocity, rule health, analyst impact?
+          <t>How many of these KPI categories does your team actively track: (1) detection coverage (ATT&amp;CK %), (2) detection quality (FP/FN rates), (3) detection velocity (time to deploy new rules), (4) rule health (stale/broken rules), (5) analyst impact (alert-to-incident ratio)?
 1 — None of these are tracked
 2 — 1 category tracked
 3 — 2-3 categories tracked with regular reporting
@@ -3057,22 +3003,21 @@
         <f>IF(E70="","",E70)</f>
         <v/>
       </c>
-      <c r="G70" s="21" t="n"/>
     </row>
     <row r="71" ht="115" customHeight="1">
-      <c r="B71" s="35" t="inlineStr">
+      <c r="B71" s="34" t="inlineStr">
         <is>
           <t>EG-Q4</t>
         </is>
       </c>
-      <c r="C71" s="36" t="inlineStr">
+      <c r="C71" s="35" t="inlineStr">
         <is>
           <t>Cross-Team Collaboration</t>
         </is>
       </c>
-      <c r="D71" s="37" t="inlineStr">
-        <is>
-          <t>Rate cross-team collaboration involving the assessed detection engineering function.
+      <c r="D71" s="36" t="inlineStr">
+        <is>
+          <t>Rate the maturity of collaboration between detection engineering and other security teams (IR, threat intel, security engineering).
 1 — Operates in isolation; no structured collaboration with other teams
 2 — Ad hoc collaboration, typically reactive to incidents or specific requests (no scheduled touchpoints)
 3 — Regular collaboration through defined channels; scheduled touchpoints at least monthly with IR and threat intel teams
@@ -3081,18 +3026,16 @@
         </is>
       </c>
       <c r="E71" s="19" t="n"/>
-      <c r="F71" s="38">
+      <c r="F71" s="37">
         <f>IF(E71="","",E71)</f>
         <v/>
       </c>
-      <c r="G71" s="21" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="25">
     <mergeCell ref="B59:F59"/>
     <mergeCell ref="B66:F66"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="B56:F56"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B48:F48"/>
@@ -3104,15 +3047,16 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B57:F57"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A2:H2"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B49:F49"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A2:G2"/>
     <mergeCell ref="B41:F41"/>
   </mergeCells>
   <conditionalFormatting sqref="F13:F71">
@@ -3155,7 +3099,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -3171,10 +3115,6 @@
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="3" customWidth="1" min="7" max="7"/>
-    <col hidden="1" width="18" customWidth="1" min="13" max="13"/>
-    <col hidden="1" width="10" customWidth="1" min="14" max="14"/>
-    <col hidden="1" width="18" customWidth="1" min="15" max="15"/>
-    <col hidden="1" width="10" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="56" customHeight="1">
@@ -3191,10 +3131,9 @@
       <c r="G1" s="2" t="n"/>
     </row>
     <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  =Assessment!D4</t>
-        </is>
+      <c r="A2" s="3">
+        <f>"  "&amp;Assessment!D4</f>
+        <v/>
       </c>
       <c r="B2" s="4" t="n"/>
       <c r="C2" s="4" t="n"/>
@@ -3202,160 +3141,52 @@
       <c r="E2" s="4" t="n"/>
       <c r="F2" s="4" t="n"/>
       <c r="G2" s="4" t="n"/>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Tier</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Dimension</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Foundation</t>
-        </is>
-      </c>
-      <c r="N3" s="40">
-        <f>D12</f>
-        <v/>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>People &amp; Organization</t>
-        </is>
-      </c>
-      <c r="P3" s="40">
-        <f>D39</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Basic</t>
-        </is>
-      </c>
-      <c r="N4" s="40">
-        <f>D17</f>
-        <v/>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Process &amp; Governance</t>
-        </is>
-      </c>
-      <c r="P4" s="40">
-        <f>D43</f>
-        <v/>
-      </c>
     </row>
     <row r="5" ht="22" customHeight="1">
-      <c r="B5" s="41" t="inlineStr">
+      <c r="B5" s="39" t="inlineStr">
         <is>
           <t>Overall Maturity Score</t>
         </is>
       </c>
-      <c r="C5" s="42" t="n"/>
-      <c r="D5" s="41" t="inlineStr">
+      <c r="C5" s="40" t="n"/>
+      <c r="D5" s="39" t="inlineStr">
         <is>
           <t>Achieved DEBMM Tier</t>
         </is>
       </c>
-      <c r="E5" s="42" t="n"/>
-      <c r="F5" s="41" t="inlineStr">
+      <c r="E5" s="40" t="n"/>
+      <c r="F5" s="39" t="inlineStr">
         <is>
           <t>Completion</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Intermediate</t>
-        </is>
-      </c>
-      <c r="N5" s="40">
-        <f>D24</f>
-        <v/>
-      </c>
     </row>
     <row r="6" ht="60" customHeight="1">
-      <c r="B6" s="43">
+      <c r="B6" s="41">
         <f>IF(COUNT(D13,D14,D15,D16,D18,D19,D20,D21,D22,D23,D25,D26,D27,D29,D30,D31,D33,D34,D40,D41,D42,D44,D45,D46)=0,"",ROUND(AVERAGE(D13,D14,D15,D16,D18,D19,D20,D21,D22,D23,D25,D26,D27,D29,D30,D31,D33,D34,D40,D41,D42,D44,D45,D46),2)&amp;" / 5.0")</f>
         <v/>
       </c>
-      <c r="C6" s="44" t="n"/>
-      <c r="D6" s="45">
+      <c r="C6" s="42" t="n"/>
+      <c r="D6" s="43">
         <f>IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3),AND(ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3,ISNUMBER(D31),D31&gt;=3),AND(ISNUMBER(D33),D33&gt;=3,ISNUMBER(D34),D34&gt;=3)),"Tier 4: Expert",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3),AND(ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3,ISNUMBER(D31),D31&gt;=3)),"Tier 3: Advanced",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3),AND(ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3)),"Tier 2: Intermediate",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3),AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3,ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3)),"Tier 1: Basic",IF(AND(AND(ISNUMBER(D13),D13&gt;=3,ISNUMBER(D14),D14&gt;=3,ISNUMBER(D15),D15&gt;=3,ISNUMBER(D16),D16&gt;=3)),"Tier 0: Foundation","Below Foundation")))))</f>
         <v/>
       </c>
-      <c r="E6" s="44" t="n"/>
-      <c r="F6" s="45">
+      <c r="E6" s="42" t="n"/>
+      <c r="F6" s="43">
         <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E24,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E35,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E43,Assessment!E44,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E50,Assessment!E51,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E61,Assessment!E62,Assessment!E63,Assessment!E64,Assessment!E65,Assessment!E68,Assessment!E69,Assessment!E70,Assessment!E71)&amp;" / 41"</f>
         <v/>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Advanced</t>
-        </is>
-      </c>
-      <c r="N6" s="40">
-        <f>D28</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" ht="8" customHeight="1">
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Expert</t>
-        </is>
-      </c>
-      <c r="N7" s="40">
-        <f>D32</f>
-        <v/>
-      </c>
-    </row>
+    </row>
+    <row r="7" ht="8" customHeight="1"/>
     <row r="8" ht="62" customHeight="1">
-      <c r="B8" s="46">
+      <c r="B8" s="44">
         <f>IF(D6="","",IF(D6="Tier 4: Expert","Your organization has achieved Tier 4 (Expert)—the highest DEBMM tier. Your detection engineering program is mature across all dimensions: proactive threat hunting, automation of key lifecycle stages, and continuous improvement driven by data. Focus on sustaining this level and contributing to the broader detection engineering community.",IF(D6="Tier 3: Advanced","Your organization has achieved Tier 3 (Advanced). You have a highly capable detection program with systematic FN reduction, external validation, and behavioral detection of advanced TTPs. To reach Tier 4, develop proactive threat hunting capabilities, adopt hypothesis-driven hunting workflows, and integrate automation and AI across the detection lifecycle.",IF(D6="Tier 2: Intermediate","Your organization has achieved Tier 2 (Intermediate). Your detection program has mature processes for rule development, telemetry management, false positive reduction, and gap analysis. To advance to Tier 3, invest in false negative triage, external validation (e.g., purple team exercises), and coverage of advanced TTPs.",IF(D6="Tier 1: Basic","Your organization has achieved Tier 1 (Basic). You have solid foundations and basic detection capabilities in place, including baseline rules, telemetry coverage, and release testing at the Defined level. To advance to Tier 2, focus on systematic false positive reduction, formal gap analysis, and internal testing and validation.",IF(D6="Tier 0: Foundation","Your organization has achieved Tier 0 (Foundation). All foundational criteria meet the Defined level, meaning you have documented processes for rule development, maintenance, roadmaps, and threat modeling. To reach Tier 1, ensure your baseline rules, telemetry quality, threat landscape reviews, and release testing also reach the Defined level.","Your organization has not yet achieved Tier 0 (Foundation). This means one or more foundational criteria—such as structured rule development, rule maintenance, roadmap documentation, or threat modeling—score below the Defined level (3.0). Focus on establishing basic, repeatable processes in these areas before advancing to higher tiers."))))))</f>
         <v/>
       </c>
-      <c r="C8" s="28" t="n"/>
-      <c r="D8" s="28" t="n"/>
-      <c r="E8" s="28" t="n"/>
-      <c r="F8" s="28" t="n"/>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Target Tier</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>Target</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Foundation</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>3</v>
-      </c>
+      <c r="C8" s="27" t="n"/>
+      <c r="D8" s="27" t="n"/>
+      <c r="E8" s="27" t="n"/>
+      <c r="F8" s="27" t="n"/>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="B10" s="15" t="inlineStr">
@@ -3367,14 +3198,6 @@
       <c r="D10" s="4" t="n"/>
       <c r="E10" s="4" t="n"/>
       <c r="F10" s="4" t="n"/>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Basic</t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="11" ht="24" customHeight="1">
       <c r="C11" s="14" t="inlineStr">
@@ -3397,669 +3220,645 @@
           <t>Status</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+    </row>
+    <row r="12" ht="28" customHeight="1">
+      <c r="C12" s="45" t="inlineStr">
+        <is>
+          <t>Foundation</t>
+        </is>
+      </c>
+      <c r="D12" s="46">
+        <f>IF(COUNT(D13,D14,D15,D16)=0,"",AVERAGE(D13,D14,D15,D16))</f>
+        <v/>
+      </c>
+      <c r="E12" s="47">
+        <f>IF(D12="","",IF(D12&gt;=4.5,"Optimized",IF(D12&gt;=3.5,"Managed",IF(D12&gt;=2.5,"Defined",IF(D12&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F12" s="47">
+        <f>IF(D12="","",IF(D12&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Structured Rule Development Approach</t>
+        </is>
+      </c>
+      <c r="D13" s="49">
+        <f>IF(COUNT(Assessment!F15,Assessment!F16)=0,"",AVERAGE(Assessment!F15,Assessment!F16))</f>
+        <v/>
+      </c>
+      <c r="E13" s="50">
+        <f>IF(D13="","",IF(D13&gt;=4.5,"Optimized",IF(D13&gt;=3.5,"Managed",IF(D13&gt;=2.5,"Defined",IF(D13&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F13" s="50">
+        <f>IF(D13="","",IF(D13&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Rule Creation and Maintenance</t>
+        </is>
+      </c>
+      <c r="D14" s="49">
+        <f>IF(COUNT(Assessment!F17)=0,"",AVERAGE(Assessment!F17))</f>
+        <v/>
+      </c>
+      <c r="E14" s="50">
+        <f>IF(D14="","",IF(D14&gt;=4.5,"Optimized",IF(D14&gt;=3.5,"Managed",IF(D14&gt;=2.5,"Defined",IF(D14&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F14" s="50">
+        <f>IF(D14="","",IF(D14&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Roadmap Documentation</t>
+        </is>
+      </c>
+      <c r="D15" s="49">
+        <f>IF(COUNT(Assessment!F18)=0,"",AVERAGE(Assessment!F18))</f>
+        <v/>
+      </c>
+      <c r="E15" s="50">
+        <f>IF(D15="","",IF(D15&gt;=4.5,"Optimized",IF(D15&gt;=3.5,"Managed",IF(D15&gt;=2.5,"Defined",IF(D15&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F15" s="50">
+        <f>IF(D15="","",IF(D15&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Threat Modeling</t>
+        </is>
+      </c>
+      <c r="D16" s="49">
+        <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21))</f>
+        <v/>
+      </c>
+      <c r="E16" s="50">
+        <f>IF(D16="","",IF(D16&gt;=4.5,"Optimized",IF(D16&gt;=3.5,"Managed",IF(D16&gt;=2.5,"Defined",IF(D16&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F16" s="50">
+        <f>IF(D16="","",IF(D16&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" ht="28" customHeight="1">
+      <c r="C17" s="45" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="D17" s="46">
+        <f>IF(COUNT(D18,D19,D20,D21,D22,D23)=0,"",AVERAGE(D18,D19,D20,D21,D22,D23))</f>
+        <v/>
+      </c>
+      <c r="E17" s="47">
+        <f>IF(D17="","",IF(D17&gt;=4.5,"Optimized",IF(D17&gt;=3.5,"Managed",IF(D17&gt;=2.5,"Defined",IF(D17&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F17" s="47">
+        <f>IF(D17="","",IF(D17&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Baseline Rule Creation</t>
+        </is>
+      </c>
+      <c r="D18" s="49">
+        <f>IF(COUNT(Assessment!F24,Assessment!F25)=0,"",AVERAGE(Assessment!F24,Assessment!F25))</f>
+        <v/>
+      </c>
+      <c r="E18" s="50">
+        <f>IF(D18="","",IF(D18&gt;=4.5,"Optimized",IF(D18&gt;=3.5,"Managed",IF(D18&gt;=2.5,"Defined",IF(D18&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F18" s="50">
+        <f>IF(D18="","",IF(D18&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Ruleset Management and Maintenance</t>
+        </is>
+      </c>
+      <c r="D19" s="49">
+        <f>IF(COUNT(Assessment!F26)=0,"",AVERAGE(Assessment!F26))</f>
+        <v/>
+      </c>
+      <c r="E19" s="50">
+        <f>IF(D19="","",IF(D19&gt;=4.5,"Optimized",IF(D19&gt;=3.5,"Managed",IF(D19&gt;=2.5,"Defined",IF(D19&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F19" s="50">
+        <f>IF(D19="","",IF(D19&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Telemetry Quality</t>
+        </is>
+      </c>
+      <c r="D20" s="49">
+        <f>IF(COUNT(Assessment!F27,Assessment!F28,Assessment!F29)=0,"",AVERAGE(Assessment!F27,Assessment!F28,Assessment!F29))</f>
+        <v/>
+      </c>
+      <c r="E20" s="50">
+        <f>IF(D20="","",IF(D20&gt;=4.5,"Optimized",IF(D20&gt;=3.5,"Managed",IF(D20&gt;=2.5,"Defined",IF(D20&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F20" s="50">
+        <f>IF(D20="","",IF(D20&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Threat Landscape Review</t>
+        </is>
+      </c>
+      <c r="D21" s="49">
+        <f>IF(COUNT(Assessment!F30)=0,"",AVERAGE(Assessment!F30))</f>
+        <v/>
+      </c>
+      <c r="E21" s="50">
+        <f>IF(D21="","",IF(D21&gt;=4.5,"Optimized",IF(D21&gt;=3.5,"Managed",IF(D21&gt;=2.5,"Defined",IF(D21&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F21" s="50">
+        <f>IF(D21="","",IF(D21&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Product Owner Engagement</t>
+        </is>
+      </c>
+      <c r="D22" s="49">
+        <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
+        <v/>
+      </c>
+      <c r="E22" s="50">
+        <f>IF(D22="","",IF(D22&gt;=4.5,"Optimized",IF(D22&gt;=3.5,"Managed",IF(D22&gt;=2.5,"Defined",IF(D22&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F22" s="50">
+        <f>IF(D22="","",IF(D22&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Release Testing and Validation</t>
+        </is>
+      </c>
+      <c r="D23" s="49">
+        <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
+        <v/>
+      </c>
+      <c r="E23" s="50">
+        <f>IF(D23="","",IF(D23&gt;=4.5,"Optimized",IF(D23&gt;=3.5,"Managed",IF(D23&gt;=2.5,"Defined",IF(D23&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F23" s="50">
+        <f>IF(D23="","",IF(D23&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" ht="28" customHeight="1">
+      <c r="C24" s="45" t="inlineStr">
         <is>
           <t>Intermediate</t>
         </is>
       </c>
-      <c r="N11" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" ht="28" customHeight="1">
-      <c r="C12" s="47" t="inlineStr">
-        <is>
-          <t>Foundation</t>
-        </is>
-      </c>
-      <c r="D12" s="48">
-        <f>IF(COUNT(D13,D14,D15,D16)=0,"",AVERAGE(D13,D14,D15,D16))</f>
-        <v/>
-      </c>
-      <c r="E12" s="49">
-        <f>IF(D12="","",IF(D12&gt;=4.5,"Optimized",IF(D12&gt;=3.5,"Managed",IF(D12&gt;=2.5,"Defined",IF(D12&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F12" s="49">
-        <f>IF(D12="","",IF(D12&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-      <c r="M12" t="inlineStr">
+      <c r="D24" s="46">
+        <f>IF(COUNT(D25,D26,D27)=0,"",AVERAGE(D25,D26,D27))</f>
+        <v/>
+      </c>
+      <c r="E24" s="47">
+        <f>IF(D24="","",IF(D24&gt;=4.5,"Optimized",IF(D24&gt;=3.5,"Managed",IF(D24&gt;=2.5,"Defined",IF(D24&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F24" s="47">
+        <f>IF(D24="","",IF(D24&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    False Positive Tuning and Reduction</t>
+        </is>
+      </c>
+      <c r="D25" s="49">
+        <f>IF(COUNT(Assessment!F35,Assessment!F36)=0,"",AVERAGE(Assessment!F35,Assessment!F36))</f>
+        <v/>
+      </c>
+      <c r="E25" s="50">
+        <f>IF(D25="","",IF(D25&gt;=4.5,"Optimized",IF(D25&gt;=3.5,"Managed",IF(D25&gt;=2.5,"Defined",IF(D25&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F25" s="50">
+        <f>IF(D25="","",IF(D25&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Gap Analysis and Documentation</t>
+        </is>
+      </c>
+      <c r="D26" s="49">
+        <f>IF(COUNT(Assessment!F37,Assessment!F38,Assessment!F39)=0,"",AVERAGE(Assessment!F37,Assessment!F38,Assessment!F39))</f>
+        <v/>
+      </c>
+      <c r="E26" s="50">
+        <f>IF(D26="","",IF(D26&gt;=4.5,"Optimized",IF(D26&gt;=3.5,"Managed",IF(D26&gt;=2.5,"Defined",IF(D26&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F26" s="50">
+        <f>IF(D26="","",IF(D26&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Internal Testing and Validation</t>
+        </is>
+      </c>
+      <c r="D27" s="49">
+        <f>IF(COUNT(Assessment!F40)=0,"",AVERAGE(Assessment!F40))</f>
+        <v/>
+      </c>
+      <c r="E27" s="50">
+        <f>IF(D27="","",IF(D27&gt;=4.5,"Optimized",IF(D27&gt;=3.5,"Managed",IF(D27&gt;=2.5,"Defined",IF(D27&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F27" s="50">
+        <f>IF(D27="","",IF(D27&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" ht="28" customHeight="1">
+      <c r="C28" s="45" t="inlineStr">
         <is>
           <t>Advanced</t>
         </is>
       </c>
-      <c r="N12" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Structured Rule Development Approach</t>
-        </is>
-      </c>
-      <c r="D13" s="51">
-        <f>IF(COUNT(Assessment!F15,Assessment!F16)=0,"",AVERAGE(Assessment!F15,Assessment!F16))</f>
-        <v/>
-      </c>
-      <c r="E13" s="52">
-        <f>IF(D13="","",IF(D13&gt;=4.5,"Optimized",IF(D13&gt;=3.5,"Managed",IF(D13&gt;=2.5,"Defined",IF(D13&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F13" s="52">
-        <f>IF(D13="","",IF(D13&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-      <c r="M13" t="inlineStr">
+      <c r="D28" s="46">
+        <f>IF(COUNT(D29,D30,D31)=0,"",AVERAGE(D29,D30,D31))</f>
+        <v/>
+      </c>
+      <c r="E28" s="47">
+        <f>IF(D28="","",IF(D28&gt;=4.5,"Optimized",IF(D28&gt;=3.5,"Managed",IF(D28&gt;=2.5,"Defined",IF(D28&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F28" s="47">
+        <f>IF(D28="","",IF(D28&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    False Negative Triage</t>
+        </is>
+      </c>
+      <c r="D29" s="49">
+        <f>IF(COUNT(Assessment!F43,Assessment!F44)=0,"",AVERAGE(Assessment!F43,Assessment!F44))</f>
+        <v/>
+      </c>
+      <c r="E29" s="50">
+        <f>IF(D29="","",IF(D29&gt;=4.5,"Optimized",IF(D29&gt;=3.5,"Managed",IF(D29&gt;=2.5,"Defined",IF(D29&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F29" s="50">
+        <f>IF(D29="","",IF(D29&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    External Validation</t>
+        </is>
+      </c>
+      <c r="D30" s="49">
+        <f>IF(COUNT(Assessment!F45)=0,"",AVERAGE(Assessment!F45))</f>
+        <v/>
+      </c>
+      <c r="E30" s="50">
+        <f>IF(D30="","",IF(D30&gt;=4.5,"Optimized",IF(D30&gt;=3.5,"Managed",IF(D30&gt;=2.5,"Defined",IF(D30&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F30" s="50">
+        <f>IF(D30="","",IF(D30&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Advanced TTP Coverage</t>
+        </is>
+      </c>
+      <c r="D31" s="49">
+        <f>IF(COUNT(Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F46,Assessment!F47))</f>
+        <v/>
+      </c>
+      <c r="E31" s="50">
+        <f>IF(D31="","",IF(D31&gt;=4.5,"Optimized",IF(D31&gt;=3.5,"Managed",IF(D31&gt;=2.5,"Defined",IF(D31&gt;=1.5,"Repeatable","Initial")))))</f>
+        <v/>
+      </c>
+      <c r="F31" s="50">
+        <f>IF(D31="","",IF(D31&gt;=3,"✓ Pass","✗ Below Target"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" ht="28" customHeight="1">
+      <c r="C32" s="45" t="inlineStr">
         <is>
           <t>Expert</t>
         </is>
       </c>
-      <c r="N13" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Rule Creation and Maintenance</t>
-        </is>
-      </c>
-      <c r="D14" s="51">
-        <f>IF(COUNT(Assessment!F17)=0,"",AVERAGE(Assessment!F17))</f>
-        <v/>
-      </c>
-      <c r="E14" s="52">
-        <f>IF(D14="","",IF(D14&gt;=4.5,"Optimized",IF(D14&gt;=3.5,"Managed",IF(D14&gt;=2.5,"Defined",IF(D14&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F14" s="52">
-        <f>IF(D14="","",IF(D14&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Roadmap Documentation</t>
-        </is>
-      </c>
-      <c r="D15" s="51">
-        <f>IF(COUNT(Assessment!F18)=0,"",AVERAGE(Assessment!F18))</f>
-        <v/>
-      </c>
-      <c r="E15" s="52">
-        <f>IF(D15="","",IF(D15&gt;=4.5,"Optimized",IF(D15&gt;=3.5,"Managed",IF(D15&gt;=2.5,"Defined",IF(D15&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F15" s="52">
-        <f>IF(D15="","",IF(D15&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Threat Modeling</t>
-        </is>
-      </c>
-      <c r="D16" s="51">
-        <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21))</f>
-        <v/>
-      </c>
-      <c r="E16" s="52">
-        <f>IF(D16="","",IF(D16&gt;=4.5,"Optimized",IF(D16&gt;=3.5,"Managed",IF(D16&gt;=2.5,"Defined",IF(D16&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F16" s="52">
-        <f>IF(D16="","",IF(D16&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" ht="28" customHeight="1">
-      <c r="C17" s="47" t="inlineStr">
-        <is>
-          <t>Basic</t>
-        </is>
-      </c>
-      <c r="D17" s="48">
-        <f>IF(COUNT(D18,D19,D20,D21,D22,D23)=0,"",AVERAGE(D18,D19,D20,D21,D22,D23))</f>
-        <v/>
-      </c>
-      <c r="E17" s="49">
-        <f>IF(D17="","",IF(D17&gt;=4.5,"Optimized",IF(D17&gt;=3.5,"Managed",IF(D17&gt;=2.5,"Defined",IF(D17&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F17" s="49">
-        <f>IF(D17="","",IF(D17&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Baseline Rule Creation</t>
-        </is>
-      </c>
-      <c r="D18" s="51">
-        <f>IF(COUNT(Assessment!F24,Assessment!F25)=0,"",AVERAGE(Assessment!F24,Assessment!F25))</f>
-        <v/>
-      </c>
-      <c r="E18" s="52">
-        <f>IF(D18="","",IF(D18&gt;=4.5,"Optimized",IF(D18&gt;=3.5,"Managed",IF(D18&gt;=2.5,"Defined",IF(D18&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F18" s="52">
-        <f>IF(D18="","",IF(D18&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Ruleset Management and Maintenance</t>
-        </is>
-      </c>
-      <c r="D19" s="51">
-        <f>IF(COUNT(Assessment!F26)=0,"",AVERAGE(Assessment!F26))</f>
-        <v/>
-      </c>
-      <c r="E19" s="52">
-        <f>IF(D19="","",IF(D19&gt;=4.5,"Optimized",IF(D19&gt;=3.5,"Managed",IF(D19&gt;=2.5,"Defined",IF(D19&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F19" s="52">
-        <f>IF(D19="","",IF(D19&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Telemetry Quality</t>
-        </is>
-      </c>
-      <c r="D20" s="51">
-        <f>IF(COUNT(Assessment!F27,Assessment!F28,Assessment!F29)=0,"",AVERAGE(Assessment!F27,Assessment!F28,Assessment!F29))</f>
-        <v/>
-      </c>
-      <c r="E20" s="52">
-        <f>IF(D20="","",IF(D20&gt;=4.5,"Optimized",IF(D20&gt;=3.5,"Managed",IF(D20&gt;=2.5,"Defined",IF(D20&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F20" s="52">
-        <f>IF(D20="","",IF(D20&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21">
-      <c r="C21" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Threat Landscape Review</t>
-        </is>
-      </c>
-      <c r="D21" s="51">
-        <f>IF(COUNT(Assessment!F30)=0,"",AVERAGE(Assessment!F30))</f>
-        <v/>
-      </c>
-      <c r="E21" s="52">
-        <f>IF(D21="","",IF(D21&gt;=4.5,"Optimized",IF(D21&gt;=3.5,"Managed",IF(D21&gt;=2.5,"Defined",IF(D21&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F21" s="52">
-        <f>IF(D21="","",IF(D21&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Product Owner Engagement</t>
-        </is>
-      </c>
-      <c r="D22" s="51">
-        <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
-        <v/>
-      </c>
-      <c r="E22" s="52">
-        <f>IF(D22="","",IF(D22&gt;=4.5,"Optimized",IF(D22&gt;=3.5,"Managed",IF(D22&gt;=2.5,"Defined",IF(D22&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F22" s="52">
-        <f>IF(D22="","",IF(D22&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Release Testing and Validation</t>
-        </is>
-      </c>
-      <c r="D23" s="51">
-        <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
-        <v/>
-      </c>
-      <c r="E23" s="52">
-        <f>IF(D23="","",IF(D23&gt;=4.5,"Optimized",IF(D23&gt;=3.5,"Managed",IF(D23&gt;=2.5,"Defined",IF(D23&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F23" s="52">
-        <f>IF(D23="","",IF(D23&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" ht="28" customHeight="1">
-      <c r="C24" s="47" t="inlineStr">
-        <is>
-          <t>Intermediate</t>
-        </is>
-      </c>
-      <c r="D24" s="48">
-        <f>IF(COUNT(D25,D26,D27)=0,"",AVERAGE(D25,D26,D27))</f>
-        <v/>
-      </c>
-      <c r="E24" s="49">
-        <f>IF(D24="","",IF(D24&gt;=4.5,"Optimized",IF(D24&gt;=3.5,"Managed",IF(D24&gt;=2.5,"Defined",IF(D24&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F24" s="49">
-        <f>IF(D24="","",IF(D24&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25">
-      <c r="C25" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    False Positive Tuning and Reduction</t>
-        </is>
-      </c>
-      <c r="D25" s="51">
-        <f>IF(COUNT(Assessment!F35,Assessment!F36)=0,"",AVERAGE(Assessment!F35,Assessment!F36))</f>
-        <v/>
-      </c>
-      <c r="E25" s="52">
-        <f>IF(D25="","",IF(D25&gt;=4.5,"Optimized",IF(D25&gt;=3.5,"Managed",IF(D25&gt;=2.5,"Defined",IF(D25&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F25" s="52">
-        <f>IF(D25="","",IF(D25&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26">
-      <c r="C26" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Gap Analysis and Documentation</t>
-        </is>
-      </c>
-      <c r="D26" s="51">
-        <f>IF(COUNT(Assessment!F37,Assessment!F38,Assessment!F39)=0,"",AVERAGE(Assessment!F37,Assessment!F38,Assessment!F39))</f>
-        <v/>
-      </c>
-      <c r="E26" s="52">
-        <f>IF(D26="","",IF(D26&gt;=4.5,"Optimized",IF(D26&gt;=3.5,"Managed",IF(D26&gt;=2.5,"Defined",IF(D26&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F26" s="52">
-        <f>IF(D26="","",IF(D26&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27">
-      <c r="C27" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Internal Testing and Validation</t>
-        </is>
-      </c>
-      <c r="D27" s="51">
-        <f>IF(COUNT(Assessment!F40)=0,"",AVERAGE(Assessment!F40))</f>
-        <v/>
-      </c>
-      <c r="E27" s="52">
-        <f>IF(D27="","",IF(D27&gt;=4.5,"Optimized",IF(D27&gt;=3.5,"Managed",IF(D27&gt;=2.5,"Defined",IF(D27&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F27" s="52">
-        <f>IF(D27="","",IF(D27&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" ht="28" customHeight="1">
-      <c r="C28" s="47" t="inlineStr">
-        <is>
-          <t>Advanced</t>
-        </is>
-      </c>
-      <c r="D28" s="48">
-        <f>IF(COUNT(D29,D30,D31)=0,"",AVERAGE(D29,D30,D31))</f>
-        <v/>
-      </c>
-      <c r="E28" s="49">
-        <f>IF(D28="","",IF(D28&gt;=4.5,"Optimized",IF(D28&gt;=3.5,"Managed",IF(D28&gt;=2.5,"Defined",IF(D28&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F28" s="49">
-        <f>IF(D28="","",IF(D28&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    False Negative Triage</t>
-        </is>
-      </c>
-      <c r="D29" s="51">
-        <f>IF(COUNT(Assessment!F43,Assessment!F44)=0,"",AVERAGE(Assessment!F43,Assessment!F44))</f>
-        <v/>
-      </c>
-      <c r="E29" s="52">
-        <f>IF(D29="","",IF(D29&gt;=4.5,"Optimized",IF(D29&gt;=3.5,"Managed",IF(D29&gt;=2.5,"Defined",IF(D29&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F29" s="52">
-        <f>IF(D29="","",IF(D29&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    External Validation</t>
-        </is>
-      </c>
-      <c r="D30" s="51">
-        <f>IF(COUNT(Assessment!F45)=0,"",AVERAGE(Assessment!F45))</f>
-        <v/>
-      </c>
-      <c r="E30" s="52">
-        <f>IF(D30="","",IF(D30&gt;=4.5,"Optimized",IF(D30&gt;=3.5,"Managed",IF(D30&gt;=2.5,"Defined",IF(D30&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F30" s="52">
-        <f>IF(D30="","",IF(D30&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31">
-      <c r="C31" s="50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    Advanced TTP Coverage</t>
-        </is>
-      </c>
-      <c r="D31" s="51">
-        <f>IF(COUNT(Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F46,Assessment!F47))</f>
-        <v/>
-      </c>
-      <c r="E31" s="52">
-        <f>IF(D31="","",IF(D31&gt;=4.5,"Optimized",IF(D31&gt;=3.5,"Managed",IF(D31&gt;=2.5,"Defined",IF(D31&gt;=1.5,"Repeatable","Initial")))))</f>
-        <v/>
-      </c>
-      <c r="F31" s="52">
-        <f>IF(D31="","",IF(D31&gt;=3,"✓ Pass","✗ Below Target"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" ht="28" customHeight="1">
-      <c r="C32" s="47" t="inlineStr">
-        <is>
-          <t>Expert</t>
-        </is>
-      </c>
-      <c r="D32" s="48">
+      <c r="D32" s="46">
         <f>IF(COUNT(D33,D34)=0,"",AVERAGE(D33,D34))</f>
         <v/>
       </c>
-      <c r="E32" s="49">
+      <c r="E32" s="47">
         <f>IF(D32="","",IF(D32&gt;=4.5,"Optimized",IF(D32&gt;=3.5,"Managed",IF(D32&gt;=2.5,"Defined",IF(D32&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F32" s="49">
+      <c r="F32" s="47">
         <f>IF(D32="","",IF(D32&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="50" t="inlineStr">
+      <c r="C33" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Threat Hunting in Telemetry</t>
         </is>
       </c>
-      <c r="D33" s="51">
+      <c r="D33" s="49">
         <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52))</f>
         <v/>
       </c>
-      <c r="E33" s="52">
+      <c r="E33" s="50">
         <f>IF(D33="","",IF(D33&gt;=4.5,"Optimized",IF(D33&gt;=3.5,"Managed",IF(D33&gt;=2.5,"Defined",IF(D33&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F33" s="52">
+      <c r="F33" s="50">
         <f>IF(D33="","",IF(D33&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="50" t="inlineStr">
+      <c r="C34" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Automation and Continuous Improvement</t>
         </is>
       </c>
-      <c r="D34" s="51">
+      <c r="D34" s="49">
         <f>IF(COUNT(Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F53,Assessment!F54))</f>
         <v/>
       </c>
-      <c r="E34" s="52">
+      <c r="E34" s="50">
         <f>IF(D34="","",IF(D34&gt;=4.5,"Optimized",IF(D34&gt;=3.5,"Managed",IF(D34&gt;=2.5,"Defined",IF(D34&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F34" s="52">
+      <c r="F34" s="50">
         <f>IF(D34="","",IF(D34&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="35" ht="14" customHeight="1">
-      <c r="A35" s="28" t="n"/>
-      <c r="B35" s="28" t="n"/>
-      <c r="C35" s="28" t="n"/>
-      <c r="D35" s="28" t="n"/>
-      <c r="E35" s="28" t="n"/>
-      <c r="F35" s="28" t="n"/>
-      <c r="G35" s="28" t="n"/>
+      <c r="A35" s="27" t="n"/>
+      <c r="B35" s="27" t="n"/>
+      <c r="C35" s="27" t="n"/>
+      <c r="D35" s="27" t="n"/>
+      <c r="E35" s="27" t="n"/>
+      <c r="F35" s="27" t="n"/>
+      <c r="G35" s="27" t="n"/>
     </row>
     <row r="36" ht="30" customHeight="1">
-      <c r="B36" s="33" t="inlineStr">
+      <c r="B36" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">  SUPPLEMENTARY DIMENSIONS</t>
         </is>
       </c>
-      <c r="C36" s="34" t="n"/>
-      <c r="D36" s="34" t="n"/>
-      <c r="E36" s="34" t="n"/>
-      <c r="F36" s="34" t="n"/>
+      <c r="C36" s="33" t="n"/>
+      <c r="D36" s="33" t="n"/>
+      <c r="E36" s="33" t="n"/>
+      <c r="F36" s="33" t="n"/>
     </row>
     <row r="37" ht="20" customHeight="1">
-      <c r="B37" s="31" t="inlineStr">
+      <c r="B37" s="30" t="inlineStr">
         <is>
           <t>Organizational readiness factors — do not affect DEBMM tier determination</t>
         </is>
       </c>
-      <c r="C37" s="30" t="n"/>
-      <c r="D37" s="30" t="n"/>
-      <c r="E37" s="30" t="n"/>
-      <c r="F37" s="30" t="n"/>
+      <c r="C37" s="29" t="n"/>
+      <c r="D37" s="29" t="n"/>
+      <c r="E37" s="29" t="n"/>
+      <c r="F37" s="29" t="n"/>
     </row>
     <row r="38" ht="24" customHeight="1">
-      <c r="C38" s="32" t="inlineStr">
+      <c r="C38" s="31" t="inlineStr">
         <is>
           <t>Category / Criterion</t>
         </is>
       </c>
-      <c r="D38" s="32" t="inlineStr">
+      <c r="D38" s="31" t="inlineStr">
         <is>
           <t>Score</t>
         </is>
       </c>
-      <c r="E38" s="32" t="inlineStr">
+      <c r="E38" s="31" t="inlineStr">
         <is>
           <t>Level</t>
         </is>
       </c>
-      <c r="F38" s="32" t="inlineStr">
+      <c r="F38" s="31" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
     </row>
     <row r="39" ht="28" customHeight="1">
-      <c r="C39" s="53" t="inlineStr">
+      <c r="C39" s="51" t="inlineStr">
         <is>
           <t>People &amp; Organization</t>
         </is>
       </c>
-      <c r="D39" s="54">
+      <c r="D39" s="52">
         <f>IF(COUNT(D40,D41,D42)=0,"",AVERAGE(D40,D41,D42))</f>
         <v/>
       </c>
-      <c r="E39" s="55">
+      <c r="E39" s="53">
         <f>IF(D39="","",IF(D39&gt;=4.5,"Optimized",IF(D39&gt;=3.5,"Managed",IF(D39&gt;=2.5,"Defined",IF(D39&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F39" s="55">
+      <c r="F39" s="53">
         <f>IF(D39="","",IF(D39&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="40">
-      <c r="C40" s="50" t="inlineStr">
+      <c r="C40" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Team Structure and Dedicated Roles</t>
         </is>
       </c>
-      <c r="D40" s="51">
+      <c r="D40" s="49">
         <f>IF(COUNT(Assessment!F61)=0,"",AVERAGE(Assessment!F61))</f>
         <v/>
       </c>
-      <c r="E40" s="52">
+      <c r="E40" s="50">
         <f>IF(D40="","",IF(D40&gt;=4.5,"Optimized",IF(D40&gt;=3.5,"Managed",IF(D40&gt;=2.5,"Defined",IF(D40&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F40" s="52">
+      <c r="F40" s="50">
         <f>IF(D40="","",IF(D40&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="41">
-      <c r="C41" s="50" t="inlineStr">
+      <c r="C41" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Skills Development and Training</t>
         </is>
       </c>
-      <c r="D41" s="51">
+      <c r="D41" s="49">
         <f>IF(COUNT(Assessment!F62)=0,"",AVERAGE(Assessment!F62))</f>
         <v/>
       </c>
-      <c r="E41" s="52">
+      <c r="E41" s="50">
         <f>IF(D41="","",IF(D41&gt;=4.5,"Optimized",IF(D41&gt;=3.5,"Managed",IF(D41&gt;=2.5,"Defined",IF(D41&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F41" s="52">
+      <c r="F41" s="50">
         <f>IF(D41="","",IF(D41&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="42">
-      <c r="C42" s="50" t="inlineStr">
+      <c r="C42" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
-      <c r="D42" s="51">
+      <c r="D42" s="49">
         <f>IF(COUNT(Assessment!F63,Assessment!F64,Assessment!F65)=0,"",AVERAGE(Assessment!F63,Assessment!F64,Assessment!F65))</f>
         <v/>
       </c>
-      <c r="E42" s="52">
+      <c r="E42" s="50">
         <f>IF(D42="","",IF(D42&gt;=4.5,"Optimized",IF(D42&gt;=3.5,"Managed",IF(D42&gt;=2.5,"Defined",IF(D42&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F42" s="52">
+      <c r="F42" s="50">
         <f>IF(D42="","",IF(D42&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="43" ht="28" customHeight="1">
-      <c r="C43" s="53" t="inlineStr">
+      <c r="C43" s="51" t="inlineStr">
         <is>
           <t>Process &amp; Governance</t>
         </is>
       </c>
-      <c r="D43" s="54">
+      <c r="D43" s="52">
         <f>IF(COUNT(D44,D45,D46)=0,"",AVERAGE(D44,D45,D46))</f>
         <v/>
       </c>
-      <c r="E43" s="55">
+      <c r="E43" s="53">
         <f>IF(D43="","",IF(D43&gt;=4.5,"Optimized",IF(D43&gt;=3.5,"Managed",IF(D43&gt;=2.5,"Defined",IF(D43&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F43" s="55">
+      <c r="F43" s="53">
         <f>IF(D43="","",IF(D43&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="44">
-      <c r="C44" s="50" t="inlineStr">
+      <c r="C44" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Detection Lifecycle Workflow</t>
         </is>
       </c>
-      <c r="D44" s="51">
+      <c r="D44" s="49">
         <f>IF(COUNT(Assessment!F68)=0,"",AVERAGE(Assessment!F68))</f>
         <v/>
       </c>
-      <c r="E44" s="52">
+      <c r="E44" s="50">
         <f>IF(D44="","",IF(D44&gt;=4.5,"Optimized",IF(D44&gt;=3.5,"Managed",IF(D44&gt;=2.5,"Defined",IF(D44&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F44" s="52">
+      <c r="F44" s="50">
         <f>IF(D44="","",IF(D44&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="45">
-      <c r="C45" s="50" t="inlineStr">
+      <c r="C45" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Metrics and KPI Tracking</t>
         </is>
       </c>
-      <c r="D45" s="51">
+      <c r="D45" s="49">
         <f>IF(COUNT(Assessment!F69,Assessment!F70)=0,"",AVERAGE(Assessment!F69,Assessment!F70))</f>
         <v/>
       </c>
-      <c r="E45" s="52">
+      <c r="E45" s="50">
         <f>IF(D45="","",IF(D45&gt;=4.5,"Optimized",IF(D45&gt;=3.5,"Managed",IF(D45&gt;=2.5,"Defined",IF(D45&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F45" s="52">
+      <c r="F45" s="50">
         <f>IF(D45="","",IF(D45&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="46">
-      <c r="C46" s="50" t="inlineStr">
+      <c r="C46" s="48" t="inlineStr">
         <is>
           <t xml:space="preserve">    Cross-Team Collaboration</t>
         </is>
       </c>
-      <c r="D46" s="51">
+      <c r="D46" s="49">
         <f>IF(COUNT(Assessment!F71)=0,"",AVERAGE(Assessment!F71))</f>
         <v/>
       </c>
-      <c r="E46" s="52">
+      <c r="E46" s="50">
         <f>IF(D46="","",IF(D46&gt;=4.5,"Optimized",IF(D46&gt;=3.5,"Managed",IF(D46&gt;=2.5,"Defined",IF(D46&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F46" s="52">
+      <c r="F46" s="50">
         <f>IF(D46="","",IF(D46&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
@@ -4148,11 +3947,341 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="003B82F6"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="3" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="3" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="48" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  DEBMM Tier Scores</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="22" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Average score per DEBMM core tier (target: 3.0)</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n"/>
+      <c r="C2" s="4" t="n"/>
+      <c r="D2" s="4" t="n"/>
+    </row>
+    <row r="4" ht="24" customHeight="1">
+      <c r="B4" s="14" t="inlineStr">
+        <is>
+          <t>Tier</t>
+        </is>
+      </c>
+      <c r="C4" s="14" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="22" customHeight="1">
+      <c r="B5" s="45" t="inlineStr">
+        <is>
+          <t>Foundation</t>
+        </is>
+      </c>
+      <c r="C5" s="54">
+        <f>'Results Dashboard'!D12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" ht="22" customHeight="1">
+      <c r="B6" s="45" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C6" s="54">
+        <f>'Results Dashboard'!D17</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" ht="22" customHeight="1">
+      <c r="B7" s="45" t="inlineStr">
+        <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="C7" s="54">
+        <f>'Results Dashboard'!D24</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" ht="22" customHeight="1">
+      <c r="B8" s="45" t="inlineStr">
+        <is>
+          <t>Advanced</t>
+        </is>
+      </c>
+      <c r="C8" s="54">
+        <f>'Results Dashboard'!D28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" ht="22" customHeight="1">
+      <c r="B9" s="45" t="inlineStr">
+        <is>
+          <t>Expert</t>
+        </is>
+      </c>
+      <c r="C9" s="54">
+        <f>'Results Dashboard'!D32</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" priority="1" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" priority="5" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" priority="9" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="12" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" priority="13" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="14" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="15" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="16" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" priority="17" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="18" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="19" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="20" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="000D7377"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="3" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="3" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="48" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Organizational Readiness</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+    </row>
+    <row r="2" ht="22" customHeight="1">
+      <c r="A2" s="55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Supplementary dimensions — do not affect DEBMM tier determination</t>
+        </is>
+      </c>
+      <c r="B2" s="33" t="n"/>
+      <c r="C2" s="33" t="n"/>
+      <c r="D2" s="33" t="n"/>
+    </row>
+    <row r="4" ht="24" customHeight="1">
+      <c r="B4" s="31" t="inlineStr">
+        <is>
+          <t>Dimension</t>
+        </is>
+      </c>
+      <c r="C4" s="31" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="22" customHeight="1">
+      <c r="B5" s="51" t="inlineStr">
+        <is>
+          <t>People &amp; Organization</t>
+        </is>
+      </c>
+      <c r="C5" s="54">
+        <f>'Results Dashboard'!D39</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" ht="22" customHeight="1">
+      <c r="B6" s="51" t="inlineStr">
+        <is>
+          <t>Process &amp; Governance</t>
+        </is>
+      </c>
+      <c r="C6" s="54">
+        <f>'Results Dashboard'!D43</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" priority="1" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" priority="5" operator="between" dxfId="0">
+      <formula>1</formula>
+      <formula>1.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="between" dxfId="1">
+      <formula>1.5</formula>
+      <formula>2.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="between" dxfId="2">
+      <formula>2.5</formula>
+      <formula>3.49</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="between" dxfId="3">
+      <formula>3.5</formula>
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="002D3E50"/>
@@ -6281,22 +6410,22 @@
     </row>
     <row r="158" ht="16" customHeight="1"/>
     <row r="159" ht="28" customHeight="1">
-      <c r="A159" s="33" t="inlineStr">
+      <c r="A159" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">  SUPPLEMENTARY DIMENSIONS</t>
         </is>
       </c>
-      <c r="B159" s="34" t="n"/>
-      <c r="C159" s="34" t="n"/>
+      <c r="B159" s="33" t="n"/>
+      <c r="C159" s="33" t="n"/>
     </row>
     <row r="160" ht="30" customHeight="1">
-      <c r="A160" s="33" t="inlineStr">
+      <c r="A160" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">  People &amp; Organization</t>
         </is>
       </c>
-      <c r="B160" s="34" t="n"/>
-      <c r="C160" s="34" t="n"/>
+      <c r="B160" s="33" t="n"/>
+      <c r="C160" s="33" t="n"/>
     </row>
     <row r="161" ht="36" customHeight="1">
       <c r="A161" s="67" t="inlineStr">
@@ -6304,17 +6433,17 @@
           <t>Assesses the human and organizational factors that enable effective detection engineering, drawn from Kyle Bailey's Detection Engineering Maturity Matrix.</t>
         </is>
       </c>
-      <c r="B161" s="30" t="n"/>
-      <c r="C161" s="30" t="n"/>
+      <c r="B161" s="29" t="n"/>
+      <c r="C161" s="29" t="n"/>
     </row>
     <row r="162" ht="26" customHeight="1">
-      <c r="A162" s="29" t="inlineStr">
+      <c r="A162" s="28" t="inlineStr">
         <is>
           <t>Team Structure and Dedicated Roles</t>
         </is>
       </c>
-      <c r="B162" s="30" t="n"/>
-      <c r="C162" s="30" t="n"/>
+      <c r="B162" s="29" t="n"/>
+      <c r="C162" s="29" t="n"/>
     </row>
     <row r="163" ht="22" customHeight="1">
       <c r="A163" s="14" t="inlineStr">
@@ -6419,13 +6548,13 @@
       </c>
     </row>
     <row r="170" ht="26" customHeight="1">
-      <c r="A170" s="29" t="inlineStr">
+      <c r="A170" s="28" t="inlineStr">
         <is>
           <t>Skills Development and Training</t>
         </is>
       </c>
-      <c r="B170" s="30" t="n"/>
-      <c r="C170" s="30" t="n"/>
+      <c r="B170" s="29" t="n"/>
+      <c r="C170" s="29" t="n"/>
     </row>
     <row r="171" ht="22" customHeight="1">
       <c r="A171" s="14" t="inlineStr">
@@ -6530,13 +6659,13 @@
       </c>
     </row>
     <row r="178" ht="26" customHeight="1">
-      <c r="A178" s="29" t="inlineStr">
+      <c r="A178" s="28" t="inlineStr">
         <is>
           <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
-      <c r="B178" s="30" t="n"/>
-      <c r="C178" s="30" t="n"/>
+      <c r="B178" s="29" t="n"/>
+      <c r="C178" s="29" t="n"/>
     </row>
     <row r="179" ht="22" customHeight="1">
       <c r="A179" s="14" t="inlineStr">
@@ -6641,13 +6770,13 @@
       </c>
     </row>
     <row r="186" ht="30" customHeight="1">
-      <c r="A186" s="33" t="inlineStr">
+      <c r="A186" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve">  Process &amp; Governance</t>
         </is>
       </c>
-      <c r="B186" s="34" t="n"/>
-      <c r="C186" s="34" t="n"/>
+      <c r="B186" s="33" t="n"/>
+      <c r="C186" s="33" t="n"/>
     </row>
     <row r="187" ht="36" customHeight="1">
       <c r="A187" s="67" t="inlineStr">
@@ -6655,17 +6784,17 @@
           <t>Assesses the process maturity and governance structures supporting detection engineering, drawn from Kyle Bailey's Detection Engineering Maturity Matrix.</t>
         </is>
       </c>
-      <c r="B187" s="30" t="n"/>
-      <c r="C187" s="30" t="n"/>
+      <c r="B187" s="29" t="n"/>
+      <c r="C187" s="29" t="n"/>
     </row>
     <row r="188" ht="26" customHeight="1">
-      <c r="A188" s="29" t="inlineStr">
+      <c r="A188" s="28" t="inlineStr">
         <is>
           <t>Detection Lifecycle Workflow</t>
         </is>
       </c>
-      <c r="B188" s="30" t="n"/>
-      <c r="C188" s="30" t="n"/>
+      <c r="B188" s="29" t="n"/>
+      <c r="C188" s="29" t="n"/>
     </row>
     <row r="189" ht="22" customHeight="1">
       <c r="A189" s="14" t="inlineStr">
@@ -6770,13 +6899,13 @@
       </c>
     </row>
     <row r="196" ht="26" customHeight="1">
-      <c r="A196" s="29" t="inlineStr">
+      <c r="A196" s="28" t="inlineStr">
         <is>
           <t>Metrics and KPI Tracking</t>
         </is>
       </c>
-      <c r="B196" s="30" t="n"/>
-      <c r="C196" s="30" t="n"/>
+      <c r="B196" s="29" t="n"/>
+      <c r="C196" s="29" t="n"/>
     </row>
     <row r="197" ht="22" customHeight="1">
       <c r="A197" s="14" t="inlineStr">
@@ -6881,13 +7010,13 @@
       </c>
     </row>
     <row r="204" ht="26" customHeight="1">
-      <c r="A204" s="29" t="inlineStr">
+      <c r="A204" s="28" t="inlineStr">
         <is>
           <t>Cross-Team Collaboration</t>
         </is>
       </c>
-      <c r="B204" s="30" t="n"/>
-      <c r="C204" s="30" t="n"/>
+      <c r="B204" s="29" t="n"/>
+      <c r="C204" s="29" t="n"/>
     </row>
     <row r="205" ht="22" customHeight="1">
       <c r="A205" s="14" t="inlineStr">
@@ -7039,7 +7168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="002D3E50"/>
@@ -7078,7 +7207,7 @@
           <t>Organization</t>
         </is>
       </c>
-      <c r="B2" s="50">
+      <c r="B2" s="48">
         <f>Assessment!D4</f>
         <v/>
       </c>
@@ -7089,7 +7218,7 @@
           <t>Assessor</t>
         </is>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="48">
         <f>Assessment!D5</f>
         <v/>
       </c>
@@ -7100,7 +7229,7 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="B4" s="50">
+      <c r="B4" s="48">
         <f>Assessment!D7</f>
         <v/>
       </c>
@@ -7111,7 +7240,7 @@
           <t>Assessment Type</t>
         </is>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="48">
         <f>Assessment!D8</f>
         <v/>
       </c>
@@ -7133,7 +7262,7 @@
           <t>Achieved Tier</t>
         </is>
       </c>
-      <c r="B7" s="50">
+      <c r="B7" s="48">
         <f>IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3),AND(ISNUMBER(D31),D31&gt;=3,ISNUMBER(D32),D32&gt;=3,ISNUMBER(D33),D33&gt;=3),AND(ISNUMBER(D34),D34&gt;=3,ISNUMBER(D35),D35&gt;=3)),"Tier 4: Expert",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3),AND(ISNUMBER(D31),D31&gt;=3,ISNUMBER(D32),D32&gt;=3,ISNUMBER(D33),D33&gt;=3)),"Tier 3: Advanced",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3),AND(ISNUMBER(D28),D28&gt;=3,ISNUMBER(D29),D29&gt;=3,ISNUMBER(D30),D30&gt;=3)),"Tier 2: Intermediate",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3),AND(ISNUMBER(D22),D22&gt;=3,ISNUMBER(D23),D23&gt;=3,ISNUMBER(D24),D24&gt;=3,ISNUMBER(D25),D25&gt;=3,ISNUMBER(D26),D26&gt;=3,ISNUMBER(D27),D27&gt;=3)),"Tier 1: Basic",IF(AND(AND(ISNUMBER(D18),D18&gt;=3,ISNUMBER(D19),D19&gt;=3,ISNUMBER(D20),D20&gt;=3,ISNUMBER(D21),D21&gt;=3)),"Tier 0: Foundation","Below Foundation")))))</f>
         <v/>
       </c>
@@ -7144,7 +7273,7 @@
           <t>Completion</t>
         </is>
       </c>
-      <c r="B8" s="50">
+      <c r="B8" s="48">
         <f>COUNTA(Assessment!E15,Assessment!E16,Assessment!E17,Assessment!E18,Assessment!E19,Assessment!E20,Assessment!E21,Assessment!E24,Assessment!E25,Assessment!E26,Assessment!E27,Assessment!E28,Assessment!E29,Assessment!E30,Assessment!E31,Assessment!E32,Assessment!E35,Assessment!E36,Assessment!E37,Assessment!E38,Assessment!E39,Assessment!E40,Assessment!E43,Assessment!E44,Assessment!E45,Assessment!E46,Assessment!E47,Assessment!E50,Assessment!E51,Assessment!E52,Assessment!E53,Assessment!E54,Assessment!E61,Assessment!E62,Assessment!E63,Assessment!E64,Assessment!E65,Assessment!E68,Assessment!E69,Assessment!E70,Assessment!E71)&amp;" / 41"</f>
         <v/>
       </c>
@@ -7192,15 +7321,15 @@
           <t>Foundation</t>
         </is>
       </c>
-      <c r="C11" s="74">
+      <c r="C11" s="54">
         <f>IF(COUNT(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F15,Assessment!F16,Assessment!F17,Assessment!F18,Assessment!F19,Assessment!F20,Assessment!F21))</f>
         <v/>
       </c>
-      <c r="D11" s="75">
+      <c r="D11" s="74">
         <f>IF(C11="","",IF(C11&gt;=4.5,"Optimized",IF(C11&gt;=3.5,"Managed",IF(C11&gt;=2.5,"Defined",IF(C11&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="E11" s="75">
+      <c r="E11" s="74">
         <f>IF(C11="","",IF(C11&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
@@ -7220,15 +7349,15 @@
           <t>Basic</t>
         </is>
       </c>
-      <c r="C12" s="74">
+      <c r="C12" s="54">
         <f>IF(COUNT(Assessment!F24,Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32)=0,"",AVERAGE(Assessment!F24,Assessment!F25,Assessment!F26,Assessment!F27,Assessment!F28,Assessment!F29,Assessment!F30,Assessment!F31,Assessment!F32))</f>
         <v/>
       </c>
-      <c r="D12" s="75">
+      <c r="D12" s="74">
         <f>IF(C12="","",IF(C12&gt;=4.5,"Optimized",IF(C12&gt;=3.5,"Managed",IF(C12&gt;=2.5,"Defined",IF(C12&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="E12" s="75">
+      <c r="E12" s="74">
         <f>IF(C12="","",IF(C12&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
@@ -7248,15 +7377,15 @@
           <t>Intermediate</t>
         </is>
       </c>
-      <c r="C13" s="74">
+      <c r="C13" s="54">
         <f>IF(COUNT(Assessment!F35,Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40)=0,"",AVERAGE(Assessment!F35,Assessment!F36,Assessment!F37,Assessment!F38,Assessment!F39,Assessment!F40))</f>
         <v/>
       </c>
-      <c r="D13" s="75">
+      <c r="D13" s="74">
         <f>IF(C13="","",IF(C13&gt;=4.5,"Optimized",IF(C13&gt;=3.5,"Managed",IF(C13&gt;=2.5,"Defined",IF(C13&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="E13" s="75">
+      <c r="E13" s="74">
         <f>IF(C13="","",IF(C13&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
@@ -7276,15 +7405,15 @@
           <t>Advanced</t>
         </is>
       </c>
-      <c r="C14" s="74">
+      <c r="C14" s="54">
         <f>IF(COUNT(Assessment!F43,Assessment!F44,Assessment!F45,Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F43,Assessment!F44,Assessment!F45,Assessment!F46,Assessment!F47))</f>
         <v/>
       </c>
-      <c r="D14" s="75">
+      <c r="D14" s="74">
         <f>IF(C14="","",IF(C14&gt;=4.5,"Optimized",IF(C14&gt;=3.5,"Managed",IF(C14&gt;=2.5,"Defined",IF(C14&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="E14" s="75">
+      <c r="E14" s="74">
         <f>IF(C14="","",IF(C14&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
@@ -7304,15 +7433,15 @@
           <t>Expert</t>
         </is>
       </c>
-      <c r="C15" s="74">
+      <c r="C15" s="54">
         <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52,Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52,Assessment!F53,Assessment!F54))</f>
         <v/>
       </c>
-      <c r="D15" s="75">
+      <c r="D15" s="74">
         <f>IF(C15="","",IF(C15&gt;=4.5,"Optimized",IF(C15&gt;=3.5,"Managed",IF(C15&gt;=2.5,"Defined",IF(C15&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="E15" s="75">
+      <c r="E15" s="74">
         <f>IF(C15="","",IF(C15&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
@@ -7354,12 +7483,12 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="50" t="inlineStr">
+      <c r="A18" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B18" s="50" t="inlineStr">
+      <c r="B18" s="48" t="inlineStr">
         <is>
           <t>Foundation</t>
         </is>
@@ -7369,26 +7498,26 @@
           <t>Structured Rule Development Approach</t>
         </is>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="49">
         <f>IF(COUNT(Assessment!F15,Assessment!F16)=0,"",AVERAGE(Assessment!F15,Assessment!F16))</f>
         <v/>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="50">
         <f>IF(D18="","",IF(D18&gt;=4.5,"Optimized",IF(D18&gt;=3.5,"Managed",IF(D18&gt;=2.5,"Defined",IF(D18&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F18" s="52">
+      <c r="F18" s="50">
         <f>IF(D18="","",IF(D18&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="50" t="inlineStr">
+      <c r="A19" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B19" s="50" t="inlineStr">
+      <c r="B19" s="48" t="inlineStr">
         <is>
           <t>Foundation</t>
         </is>
@@ -7398,26 +7527,26 @@
           <t>Rule Creation and Maintenance</t>
         </is>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="49">
         <f>IF(COUNT(Assessment!F17)=0,"",AVERAGE(Assessment!F17))</f>
         <v/>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="50">
         <f>IF(D19="","",IF(D19&gt;=4.5,"Optimized",IF(D19&gt;=3.5,"Managed",IF(D19&gt;=2.5,"Defined",IF(D19&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F19" s="52">
+      <c r="F19" s="50">
         <f>IF(D19="","",IF(D19&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="50" t="inlineStr">
+      <c r="A20" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B20" s="50" t="inlineStr">
+      <c r="B20" s="48" t="inlineStr">
         <is>
           <t>Foundation</t>
         </is>
@@ -7427,26 +7556,26 @@
           <t>Roadmap Documentation</t>
         </is>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="49">
         <f>IF(COUNT(Assessment!F18)=0,"",AVERAGE(Assessment!F18))</f>
         <v/>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="50">
         <f>IF(D20="","",IF(D20&gt;=4.5,"Optimized",IF(D20&gt;=3.5,"Managed",IF(D20&gt;=2.5,"Defined",IF(D20&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="50">
         <f>IF(D20="","",IF(D20&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="50" t="inlineStr">
+      <c r="A21" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B21" s="50" t="inlineStr">
+      <c r="B21" s="48" t="inlineStr">
         <is>
           <t>Foundation</t>
         </is>
@@ -7456,26 +7585,26 @@
           <t>Threat Modeling</t>
         </is>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="49">
         <f>IF(COUNT(Assessment!F19,Assessment!F20,Assessment!F21)=0,"",AVERAGE(Assessment!F19,Assessment!F20,Assessment!F21))</f>
         <v/>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="50">
         <f>IF(D21="","",IF(D21&gt;=4.5,"Optimized",IF(D21&gt;=3.5,"Managed",IF(D21&gt;=2.5,"Defined",IF(D21&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="50">
         <f>IF(D21="","",IF(D21&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="50" t="inlineStr">
+      <c r="A22" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B22" s="50" t="inlineStr">
+      <c r="B22" s="48" t="inlineStr">
         <is>
           <t>Basic</t>
         </is>
@@ -7485,26 +7614,26 @@
           <t>Baseline Rule Creation</t>
         </is>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="49">
         <f>IF(COUNT(Assessment!F24,Assessment!F25)=0,"",AVERAGE(Assessment!F24,Assessment!F25))</f>
         <v/>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="50">
         <f>IF(D22="","",IF(D22&gt;=4.5,"Optimized",IF(D22&gt;=3.5,"Managed",IF(D22&gt;=2.5,"Defined",IF(D22&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F22" s="52">
+      <c r="F22" s="50">
         <f>IF(D22="","",IF(D22&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="50" t="inlineStr">
+      <c r="A23" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B23" s="50" t="inlineStr">
+      <c r="B23" s="48" t="inlineStr">
         <is>
           <t>Basic</t>
         </is>
@@ -7514,26 +7643,26 @@
           <t>Ruleset Management and Maintenance</t>
         </is>
       </c>
-      <c r="D23" s="51">
+      <c r="D23" s="49">
         <f>IF(COUNT(Assessment!F26)=0,"",AVERAGE(Assessment!F26))</f>
         <v/>
       </c>
-      <c r="E23" s="52">
+      <c r="E23" s="50">
         <f>IF(D23="","",IF(D23&gt;=4.5,"Optimized",IF(D23&gt;=3.5,"Managed",IF(D23&gt;=2.5,"Defined",IF(D23&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F23" s="52">
+      <c r="F23" s="50">
         <f>IF(D23="","",IF(D23&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="50" t="inlineStr">
+      <c r="A24" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B24" s="50" t="inlineStr">
+      <c r="B24" s="48" t="inlineStr">
         <is>
           <t>Basic</t>
         </is>
@@ -7543,26 +7672,26 @@
           <t>Telemetry Quality</t>
         </is>
       </c>
-      <c r="D24" s="51">
+      <c r="D24" s="49">
         <f>IF(COUNT(Assessment!F27,Assessment!F28,Assessment!F29)=0,"",AVERAGE(Assessment!F27,Assessment!F28,Assessment!F29))</f>
         <v/>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="50">
         <f>IF(D24="","",IF(D24&gt;=4.5,"Optimized",IF(D24&gt;=3.5,"Managed",IF(D24&gt;=2.5,"Defined",IF(D24&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="50">
         <f>IF(D24="","",IF(D24&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="50" t="inlineStr">
+      <c r="A25" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B25" s="50" t="inlineStr">
+      <c r="B25" s="48" t="inlineStr">
         <is>
           <t>Basic</t>
         </is>
@@ -7572,26 +7701,26 @@
           <t>Threat Landscape Review</t>
         </is>
       </c>
-      <c r="D25" s="51">
+      <c r="D25" s="49">
         <f>IF(COUNT(Assessment!F30)=0,"",AVERAGE(Assessment!F30))</f>
         <v/>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="50">
         <f>IF(D25="","",IF(D25&gt;=4.5,"Optimized",IF(D25&gt;=3.5,"Managed",IF(D25&gt;=2.5,"Defined",IF(D25&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F25" s="52">
+      <c r="F25" s="50">
         <f>IF(D25="","",IF(D25&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="50" t="inlineStr">
+      <c r="A26" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B26" s="50" t="inlineStr">
+      <c r="B26" s="48" t="inlineStr">
         <is>
           <t>Basic</t>
         </is>
@@ -7601,26 +7730,26 @@
           <t>Product Owner Engagement</t>
         </is>
       </c>
-      <c r="D26" s="51">
+      <c r="D26" s="49">
         <f>IF(COUNT(Assessment!F31)=0,"",AVERAGE(Assessment!F31))</f>
         <v/>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="50">
         <f>IF(D26="","",IF(D26&gt;=4.5,"Optimized",IF(D26&gt;=3.5,"Managed",IF(D26&gt;=2.5,"Defined",IF(D26&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F26" s="52">
+      <c r="F26" s="50">
         <f>IF(D26="","",IF(D26&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="50" t="inlineStr">
+      <c r="A27" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B27" s="50" t="inlineStr">
+      <c r="B27" s="48" t="inlineStr">
         <is>
           <t>Basic</t>
         </is>
@@ -7630,26 +7759,26 @@
           <t>Release Testing and Validation</t>
         </is>
       </c>
-      <c r="D27" s="51">
+      <c r="D27" s="49">
         <f>IF(COUNT(Assessment!F32)=0,"",AVERAGE(Assessment!F32))</f>
         <v/>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="50">
         <f>IF(D27="","",IF(D27&gt;=4.5,"Optimized",IF(D27&gt;=3.5,"Managed",IF(D27&gt;=2.5,"Defined",IF(D27&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F27" s="52">
+      <c r="F27" s="50">
         <f>IF(D27="","",IF(D27&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="50" t="inlineStr">
+      <c r="A28" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B28" s="50" t="inlineStr">
+      <c r="B28" s="48" t="inlineStr">
         <is>
           <t>Intermediate</t>
         </is>
@@ -7659,26 +7788,26 @@
           <t>False Positive Tuning and Reduction</t>
         </is>
       </c>
-      <c r="D28" s="51">
+      <c r="D28" s="49">
         <f>IF(COUNT(Assessment!F35,Assessment!F36)=0,"",AVERAGE(Assessment!F35,Assessment!F36))</f>
         <v/>
       </c>
-      <c r="E28" s="52">
+      <c r="E28" s="50">
         <f>IF(D28="","",IF(D28&gt;=4.5,"Optimized",IF(D28&gt;=3.5,"Managed",IF(D28&gt;=2.5,"Defined",IF(D28&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F28" s="52">
+      <c r="F28" s="50">
         <f>IF(D28="","",IF(D28&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="50" t="inlineStr">
+      <c r="A29" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B29" s="50" t="inlineStr">
+      <c r="B29" s="48" t="inlineStr">
         <is>
           <t>Intermediate</t>
         </is>
@@ -7688,26 +7817,26 @@
           <t>Gap Analysis and Documentation</t>
         </is>
       </c>
-      <c r="D29" s="51">
+      <c r="D29" s="49">
         <f>IF(COUNT(Assessment!F37,Assessment!F38,Assessment!F39)=0,"",AVERAGE(Assessment!F37,Assessment!F38,Assessment!F39))</f>
         <v/>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="50">
         <f>IF(D29="","",IF(D29&gt;=4.5,"Optimized",IF(D29&gt;=3.5,"Managed",IF(D29&gt;=2.5,"Defined",IF(D29&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F29" s="52">
+      <c r="F29" s="50">
         <f>IF(D29="","",IF(D29&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="50" t="inlineStr">
+      <c r="A30" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B30" s="50" t="inlineStr">
+      <c r="B30" s="48" t="inlineStr">
         <is>
           <t>Intermediate</t>
         </is>
@@ -7717,26 +7846,26 @@
           <t>Internal Testing and Validation</t>
         </is>
       </c>
-      <c r="D30" s="51">
+      <c r="D30" s="49">
         <f>IF(COUNT(Assessment!F40)=0,"",AVERAGE(Assessment!F40))</f>
         <v/>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="50">
         <f>IF(D30="","",IF(D30&gt;=4.5,"Optimized",IF(D30&gt;=3.5,"Managed",IF(D30&gt;=2.5,"Defined",IF(D30&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F30" s="52">
+      <c r="F30" s="50">
         <f>IF(D30="","",IF(D30&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="50" t="inlineStr">
+      <c r="A31" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B31" s="50" t="inlineStr">
+      <c r="B31" s="48" t="inlineStr">
         <is>
           <t>Advanced</t>
         </is>
@@ -7746,26 +7875,26 @@
           <t>False Negative Triage</t>
         </is>
       </c>
-      <c r="D31" s="51">
+      <c r="D31" s="49">
         <f>IF(COUNT(Assessment!F43,Assessment!F44)=0,"",AVERAGE(Assessment!F43,Assessment!F44))</f>
         <v/>
       </c>
-      <c r="E31" s="52">
+      <c r="E31" s="50">
         <f>IF(D31="","",IF(D31&gt;=4.5,"Optimized",IF(D31&gt;=3.5,"Managed",IF(D31&gt;=2.5,"Defined",IF(D31&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F31" s="52">
+      <c r="F31" s="50">
         <f>IF(D31="","",IF(D31&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="50" t="inlineStr">
+      <c r="A32" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B32" s="50" t="inlineStr">
+      <c r="B32" s="48" t="inlineStr">
         <is>
           <t>Advanced</t>
         </is>
@@ -7775,26 +7904,26 @@
           <t>External Validation</t>
         </is>
       </c>
-      <c r="D32" s="51">
+      <c r="D32" s="49">
         <f>IF(COUNT(Assessment!F45)=0,"",AVERAGE(Assessment!F45))</f>
         <v/>
       </c>
-      <c r="E32" s="52">
+      <c r="E32" s="50">
         <f>IF(D32="","",IF(D32&gt;=4.5,"Optimized",IF(D32&gt;=3.5,"Managed",IF(D32&gt;=2.5,"Defined",IF(D32&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F32" s="52">
+      <c r="F32" s="50">
         <f>IF(D32="","",IF(D32&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="50" t="inlineStr">
+      <c r="A33" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B33" s="50" t="inlineStr">
+      <c r="B33" s="48" t="inlineStr">
         <is>
           <t>Advanced</t>
         </is>
@@ -7804,26 +7933,26 @@
           <t>Advanced TTP Coverage</t>
         </is>
       </c>
-      <c r="D33" s="51">
+      <c r="D33" s="49">
         <f>IF(COUNT(Assessment!F46,Assessment!F47)=0,"",AVERAGE(Assessment!F46,Assessment!F47))</f>
         <v/>
       </c>
-      <c r="E33" s="52">
+      <c r="E33" s="50">
         <f>IF(D33="","",IF(D33&gt;=4.5,"Optimized",IF(D33&gt;=3.5,"Managed",IF(D33&gt;=2.5,"Defined",IF(D33&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F33" s="52">
+      <c r="F33" s="50">
         <f>IF(D33="","",IF(D33&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="50" t="inlineStr">
+      <c r="A34" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B34" s="50" t="inlineStr">
+      <c r="B34" s="48" t="inlineStr">
         <is>
           <t>Expert</t>
         </is>
@@ -7833,26 +7962,26 @@
           <t>Threat Hunting in Telemetry</t>
         </is>
       </c>
-      <c r="D34" s="51">
+      <c r="D34" s="49">
         <f>IF(COUNT(Assessment!F50,Assessment!F51,Assessment!F52)=0,"",AVERAGE(Assessment!F50,Assessment!F51,Assessment!F52))</f>
         <v/>
       </c>
-      <c r="E34" s="52">
+      <c r="E34" s="50">
         <f>IF(D34="","",IF(D34&gt;=4.5,"Optimized",IF(D34&gt;=3.5,"Managed",IF(D34&gt;=2.5,"Defined",IF(D34&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F34" s="52">
+      <c r="F34" s="50">
         <f>IF(D34="","",IF(D34&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="50" t="inlineStr">
+      <c r="A35" s="48" t="inlineStr">
         <is>
           <t>DEBMM Core</t>
         </is>
       </c>
-      <c r="B35" s="50" t="inlineStr">
+      <c r="B35" s="48" t="inlineStr">
         <is>
           <t>Expert</t>
         </is>
@@ -7862,26 +7991,26 @@
           <t>Automation and Continuous Improvement</t>
         </is>
       </c>
-      <c r="D35" s="51">
+      <c r="D35" s="49">
         <f>IF(COUNT(Assessment!F53,Assessment!F54)=0,"",AVERAGE(Assessment!F53,Assessment!F54))</f>
         <v/>
       </c>
-      <c r="E35" s="52">
+      <c r="E35" s="50">
         <f>IF(D35="","",IF(D35&gt;=4.5,"Optimized",IF(D35&gt;=3.5,"Managed",IF(D35&gt;=2.5,"Defined",IF(D35&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F35" s="52">
+      <c r="F35" s="50">
         <f>IF(D35="","",IF(D35&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="50" t="inlineStr">
+      <c r="A36" s="48" t="inlineStr">
         <is>
           <t>Enrichment</t>
         </is>
       </c>
-      <c r="B36" s="50" t="inlineStr">
+      <c r="B36" s="48" t="inlineStr">
         <is>
           <t>People &amp; Organization</t>
         </is>
@@ -7891,26 +8020,26 @@
           <t>Team Structure and Dedicated Roles</t>
         </is>
       </c>
-      <c r="D36" s="51">
+      <c r="D36" s="49">
         <f>IF(COUNT(Assessment!F61)=0,"",AVERAGE(Assessment!F61))</f>
         <v/>
       </c>
-      <c r="E36" s="52">
+      <c r="E36" s="50">
         <f>IF(D36="","",IF(D36&gt;=4.5,"Optimized",IF(D36&gt;=3.5,"Managed",IF(D36&gt;=2.5,"Defined",IF(D36&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F36" s="52">
+      <c r="F36" s="50">
         <f>IF(D36="","",IF(D36&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="50" t="inlineStr">
+      <c r="A37" s="48" t="inlineStr">
         <is>
           <t>Enrichment</t>
         </is>
       </c>
-      <c r="B37" s="50" t="inlineStr">
+      <c r="B37" s="48" t="inlineStr">
         <is>
           <t>People &amp; Organization</t>
         </is>
@@ -7920,26 +8049,26 @@
           <t>Skills Development and Training</t>
         </is>
       </c>
-      <c r="D37" s="51">
+      <c r="D37" s="49">
         <f>IF(COUNT(Assessment!F62)=0,"",AVERAGE(Assessment!F62))</f>
         <v/>
       </c>
-      <c r="E37" s="52">
+      <c r="E37" s="50">
         <f>IF(D37="","",IF(D37&gt;=4.5,"Optimized",IF(D37&gt;=3.5,"Managed",IF(D37&gt;=2.5,"Defined",IF(D37&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F37" s="52">
+      <c r="F37" s="50">
         <f>IF(D37="","",IF(D37&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="50" t="inlineStr">
+      <c r="A38" s="48" t="inlineStr">
         <is>
           <t>Enrichment</t>
         </is>
       </c>
-      <c r="B38" s="50" t="inlineStr">
+      <c r="B38" s="48" t="inlineStr">
         <is>
           <t>People &amp; Organization</t>
         </is>
@@ -7949,26 +8078,26 @@
           <t>Leadership Commitment and Executive Sponsorship</t>
         </is>
       </c>
-      <c r="D38" s="51">
+      <c r="D38" s="49">
         <f>IF(COUNT(Assessment!F63,Assessment!F64,Assessment!F65)=0,"",AVERAGE(Assessment!F63,Assessment!F64,Assessment!F65))</f>
         <v/>
       </c>
-      <c r="E38" s="52">
+      <c r="E38" s="50">
         <f>IF(D38="","",IF(D38&gt;=4.5,"Optimized",IF(D38&gt;=3.5,"Managed",IF(D38&gt;=2.5,"Defined",IF(D38&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F38" s="52">
+      <c r="F38" s="50">
         <f>IF(D38="","",IF(D38&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="50" t="inlineStr">
+      <c r="A39" s="48" t="inlineStr">
         <is>
           <t>Enrichment</t>
         </is>
       </c>
-      <c r="B39" s="50" t="inlineStr">
+      <c r="B39" s="48" t="inlineStr">
         <is>
           <t>Process &amp; Governance</t>
         </is>
@@ -7978,26 +8107,26 @@
           <t>Detection Lifecycle Workflow</t>
         </is>
       </c>
-      <c r="D39" s="51">
+      <c r="D39" s="49">
         <f>IF(COUNT(Assessment!F68)=0,"",AVERAGE(Assessment!F68))</f>
         <v/>
       </c>
-      <c r="E39" s="52">
+      <c r="E39" s="50">
         <f>IF(D39="","",IF(D39&gt;=4.5,"Optimized",IF(D39&gt;=3.5,"Managed",IF(D39&gt;=2.5,"Defined",IF(D39&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F39" s="52">
+      <c r="F39" s="50">
         <f>IF(D39="","",IF(D39&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="50" t="inlineStr">
+      <c r="A40" s="48" t="inlineStr">
         <is>
           <t>Enrichment</t>
         </is>
       </c>
-      <c r="B40" s="50" t="inlineStr">
+      <c r="B40" s="48" t="inlineStr">
         <is>
           <t>Process &amp; Governance</t>
         </is>
@@ -8007,26 +8136,26 @@
           <t>Metrics and KPI Tracking</t>
         </is>
       </c>
-      <c r="D40" s="51">
+      <c r="D40" s="49">
         <f>IF(COUNT(Assessment!F69,Assessment!F70)=0,"",AVERAGE(Assessment!F69,Assessment!F70))</f>
         <v/>
       </c>
-      <c r="E40" s="52">
+      <c r="E40" s="50">
         <f>IF(D40="","",IF(D40&gt;=4.5,"Optimized",IF(D40&gt;=3.5,"Managed",IF(D40&gt;=2.5,"Defined",IF(D40&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F40" s="52">
+      <c r="F40" s="50">
         <f>IF(D40="","",IF(D40&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="50" t="inlineStr">
+      <c r="A41" s="48" t="inlineStr">
         <is>
           <t>Enrichment</t>
         </is>
       </c>
-      <c r="B41" s="50" t="inlineStr">
+      <c r="B41" s="48" t="inlineStr">
         <is>
           <t>Process &amp; Governance</t>
         </is>
@@ -8036,15 +8165,15 @@
           <t>Cross-Team Collaboration</t>
         </is>
       </c>
-      <c r="D41" s="51">
+      <c r="D41" s="49">
         <f>IF(COUNT(Assessment!F71)=0,"",AVERAGE(Assessment!F71))</f>
         <v/>
       </c>
-      <c r="E41" s="52">
+      <c r="E41" s="50">
         <f>IF(D41="","",IF(D41&gt;=4.5,"Optimized",IF(D41&gt;=3.5,"Managed",IF(D41&gt;=2.5,"Defined",IF(D41&gt;=1.5,"Repeatable","Initial")))))</f>
         <v/>
       </c>
-      <c r="F41" s="52">
+      <c r="F41" s="50">
         <f>IF(D41="","",IF(D41&gt;=3,"✓ Pass","✗ Below Target"))</f>
         <v/>
       </c>

</xml_diff>